<commit_message>
Starting training requirement tests code
</commit_message>
<xml_diff>
--- a/Code/R/litresults.xlsx
+++ b/Code/R/litresults.xlsx
@@ -2,9 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
-  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="460" yWindow="1020" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -406,7 +406,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -440,6 +440,13 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
@@ -1831,11 +1838,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:AA506"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A475" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E500" sqref="E500"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A459" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="W496" sqref="W496"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -11759,14 +11769,14 @@
       <c r="M257" s="1">
         <v>-5</v>
       </c>
-      <c r="R257" s="1">
+      <c r="R257" s="2">
         <f>S257-1.3586</f>
         <v>8.2999999999999963E-2</v>
       </c>
       <c r="S257" s="1">
         <v>1.4416</v>
       </c>
-      <c r="V257" s="1">
+      <c r="V257" s="2">
         <f>W257-0.5454</f>
         <v>0.121</v>
       </c>
@@ -11802,14 +11812,14 @@
       <c r="M258" s="1">
         <v>0</v>
       </c>
-      <c r="R258" s="1">
+      <c r="R258" s="2">
         <f>S258-1.6189</f>
         <v>0.2004999999999999</v>
       </c>
       <c r="S258" s="1">
         <v>1.8193999999999999</v>
       </c>
-      <c r="V258" s="1">
+      <c r="V258" s="2">
         <f>W258-0.6561</f>
         <v>0.11880000000000002</v>
       </c>
@@ -11845,14 +11855,14 @@
       <c r="M259" s="1">
         <v>-5</v>
       </c>
-      <c r="R259" s="1">
+      <c r="R259" s="2">
         <f>S259-1.3586</f>
         <v>0.48580000000000001</v>
       </c>
       <c r="S259" s="1">
         <v>1.8444</v>
       </c>
-      <c r="V259" s="1">
+      <c r="V259" s="2">
         <f>W259-0.5454</f>
         <v>0.15820000000000001</v>
       </c>
@@ -11888,14 +11898,14 @@
       <c r="M260" s="1">
         <v>0</v>
       </c>
-      <c r="R260" s="1">
+      <c r="R260" s="2">
         <f>S260-1.6189</f>
         <v>0.54389999999999983</v>
       </c>
       <c r="S260" s="1">
         <v>2.1627999999999998</v>
       </c>
-      <c r="V260" s="1">
+      <c r="V260" s="2">
         <f>W260-0.6561</f>
         <v>0.1512</v>
       </c>
@@ -11931,14 +11941,14 @@
       <c r="M261" s="1">
         <v>-5</v>
       </c>
-      <c r="R261" s="1">
+      <c r="R261" s="2">
         <f>S261-1.3586</f>
         <v>0.29489999999999994</v>
       </c>
       <c r="S261" s="1">
         <v>1.6535</v>
       </c>
-      <c r="V261" s="1">
+      <c r="V261" s="2">
         <f>W261-0.5454</f>
         <v>3.6800000000000055E-2</v>
       </c>
@@ -11974,14 +11984,14 @@
       <c r="M262" s="1">
         <v>0</v>
       </c>
-      <c r="R262" s="1">
+      <c r="R262" s="2">
         <f>S262-1.6189</f>
         <v>0.34939999999999993</v>
       </c>
       <c r="S262" s="1">
         <v>1.9682999999999999</v>
       </c>
-      <c r="V262" s="1">
+      <c r="V262" s="2">
         <f>W262-0.6561</f>
         <v>4.0599999999999969E-2</v>
       </c>
@@ -12017,14 +12027,14 @@
       <c r="M263" s="1">
         <v>-5</v>
       </c>
-      <c r="R263" s="1">
+      <c r="R263" s="2">
         <f>S263-1.3586</f>
         <v>0.15419999999999989</v>
       </c>
       <c r="S263" s="1">
         <v>1.5127999999999999</v>
       </c>
-      <c r="V263" s="1">
+      <c r="V263" s="2">
         <f>W263-0.5454</f>
         <v>1.8199999999999994E-2</v>
       </c>
@@ -12060,14 +12070,14 @@
       <c r="M264" s="1">
         <v>0</v>
       </c>
-      <c r="R264" s="1">
+      <c r="R264" s="2">
         <f>S264-1.6189</f>
         <v>0.18080000000000007</v>
       </c>
       <c r="S264" s="1">
         <v>1.7997000000000001</v>
       </c>
-      <c r="V264" s="1">
+      <c r="V264" s="2">
         <f>W264-0.6561</f>
         <v>2.1900000000000031E-2</v>
       </c>
@@ -12100,14 +12110,14 @@
       <c r="M265" s="1">
         <v>0</v>
       </c>
-      <c r="R265" s="1">
+      <c r="R265" s="2">
         <f>S265-1.55</f>
         <v>0.22999999999999998</v>
       </c>
       <c r="S265" s="1">
         <v>1.78</v>
       </c>
-      <c r="Z265" s="1">
+      <c r="Z265" s="2">
         <f>AA265-0.1411</f>
         <v>0.11299999999999999</v>
       </c>
@@ -12140,14 +12150,14 @@
       <c r="M266" s="1">
         <v>0</v>
       </c>
-      <c r="R266" s="1">
+      <c r="R266" s="2">
         <f t="shared" ref="R266:R280" si="3">S266-1.55</f>
         <v>6.0000000000000053E-2</v>
       </c>
       <c r="S266" s="1">
         <v>1.61</v>
       </c>
-      <c r="Z266" s="1">
+      <c r="Z266" s="2">
         <f>AA266-0.1411</f>
         <v>2.1500000000000019E-2</v>
       </c>
@@ -12180,14 +12190,14 @@
       <c r="M267" s="1">
         <v>0</v>
       </c>
-      <c r="R267" s="1">
+      <c r="R267" s="2">
         <f t="shared" si="3"/>
         <v>6.0000000000000053E-2</v>
       </c>
       <c r="S267" s="1">
         <v>1.61</v>
       </c>
-      <c r="Z267" s="1">
+      <c r="Z267" s="2">
         <f>AA267-0.1411</f>
         <v>1.6399999999999998E-2</v>
       </c>
@@ -12220,14 +12230,14 @@
       <c r="M268" s="1">
         <v>0</v>
       </c>
-      <c r="R268" s="1">
+      <c r="R268" s="2">
         <f t="shared" si="3"/>
         <v>0.45999999999999974</v>
       </c>
       <c r="S268" s="1">
         <v>2.0099999999999998</v>
       </c>
-      <c r="Z268" s="1">
+      <c r="Z268" s="2">
         <f t="shared" ref="Z268:Z280" si="4">AA268-0.1411</f>
         <v>0.1678</v>
       </c>
@@ -12260,14 +12270,14 @@
       <c r="M269" s="1">
         <v>0</v>
       </c>
-      <c r="R269" s="1">
+      <c r="R269" s="2">
         <f t="shared" si="3"/>
         <v>0.22999999999999998</v>
       </c>
       <c r="S269" s="1">
         <v>1.78</v>
       </c>
-      <c r="Z269" s="1">
+      <c r="Z269" s="2">
         <f t="shared" si="4"/>
         <v>-5.3400000000000003E-2</v>
       </c>
@@ -12300,14 +12310,14 @@
       <c r="M270" s="1">
         <v>0</v>
       </c>
-      <c r="R270" s="1">
+      <c r="R270" s="2">
         <f t="shared" si="3"/>
         <v>0.49</v>
       </c>
       <c r="S270" s="1">
         <v>2.04</v>
       </c>
-      <c r="Z270" s="1">
+      <c r="Z270" s="2">
         <f t="shared" si="4"/>
         <v>8.9900000000000008E-2</v>
       </c>
@@ -12340,14 +12350,14 @@
       <c r="M271" s="1">
         <v>0</v>
       </c>
-      <c r="R271" s="1">
+      <c r="R271" s="2">
         <f t="shared" si="3"/>
         <v>0.59000000000000008</v>
       </c>
       <c r="S271" s="1">
         <v>2.14</v>
       </c>
-      <c r="Z271" s="1">
+      <c r="Z271" s="2">
         <f t="shared" si="4"/>
         <v>0.18459999999999999</v>
       </c>
@@ -12380,14 +12390,14 @@
       <c r="M272" s="1">
         <v>0</v>
       </c>
-      <c r="R272" s="1">
+      <c r="R272" s="2">
         <f t="shared" si="3"/>
         <v>0.57999999999999985</v>
       </c>
       <c r="S272" s="1">
         <v>2.13</v>
       </c>
-      <c r="Z272" s="1">
+      <c r="Z272" s="2">
         <f t="shared" si="4"/>
         <v>0.1346</v>
       </c>
@@ -12420,14 +12430,14 @@
       <c r="M273" s="1">
         <v>0</v>
       </c>
-      <c r="R273" s="1">
+      <c r="R273" s="2">
         <f t="shared" si="3"/>
         <v>0.40999999999999992</v>
       </c>
       <c r="S273" s="1">
         <v>1.96</v>
       </c>
-      <c r="Z273" s="1">
+      <c r="Z273" s="2">
         <f t="shared" si="4"/>
         <v>0.19140000000000001</v>
       </c>
@@ -12460,14 +12470,14 @@
       <c r="M274" s="1">
         <v>0</v>
       </c>
-      <c r="R274" s="1">
+      <c r="R274" s="2">
         <f t="shared" si="3"/>
         <v>0.3899999999999999</v>
       </c>
       <c r="S274" s="1">
         <v>1.94</v>
       </c>
-      <c r="Z274" s="1">
+      <c r="Z274" s="2">
         <f t="shared" si="4"/>
         <v>0.18020000000000003</v>
       </c>
@@ -12500,14 +12510,14 @@
       <c r="M275" s="1">
         <v>0</v>
       </c>
-      <c r="R275" s="1">
+      <c r="R275" s="2">
         <f t="shared" si="3"/>
         <v>0.55999999999999983</v>
       </c>
       <c r="S275" s="1">
         <v>2.11</v>
       </c>
-      <c r="Z275" s="1">
+      <c r="Z275" s="2">
         <f t="shared" si="4"/>
         <v>0.18780000000000002</v>
       </c>
@@ -12540,14 +12550,14 @@
       <c r="M276" s="1">
         <v>0</v>
       </c>
-      <c r="R276" s="1">
+      <c r="R276" s="2">
         <f t="shared" si="3"/>
         <v>9.9999999999999867E-2</v>
       </c>
       <c r="S276" s="1">
         <v>1.65</v>
       </c>
-      <c r="Z276" s="1">
+      <c r="Z276" s="2">
         <f t="shared" si="4"/>
         <v>0.15359999999999996</v>
       </c>
@@ -12580,14 +12590,14 @@
       <c r="M277" s="1">
         <v>0</v>
       </c>
-      <c r="R277" s="1">
+      <c r="R277" s="2">
         <f t="shared" si="3"/>
         <v>0.55999999999999983</v>
       </c>
       <c r="S277" s="1">
         <v>2.11</v>
       </c>
-      <c r="Z277" s="1">
+      <c r="Z277" s="2">
         <f t="shared" si="4"/>
         <v>0.18549999999999994</v>
       </c>
@@ -12620,14 +12630,14 @@
       <c r="M278" s="1">
         <v>0</v>
       </c>
-      <c r="R278" s="1">
+      <c r="R278" s="2">
         <f t="shared" si="3"/>
         <v>0.59999999999999987</v>
       </c>
       <c r="S278" s="1">
         <v>2.15</v>
       </c>
-      <c r="Z278" s="1">
+      <c r="Z278" s="2">
         <f t="shared" si="4"/>
         <v>0.21950000000000003</v>
       </c>
@@ -12660,14 +12670,14 @@
       <c r="M279" s="1">
         <v>0</v>
       </c>
-      <c r="R279" s="1">
+      <c r="R279" s="2">
         <f t="shared" si="3"/>
         <v>0.61999999999999988</v>
       </c>
       <c r="S279" s="1">
         <v>2.17</v>
       </c>
-      <c r="Z279" s="1">
+      <c r="Z279" s="2">
         <f t="shared" si="4"/>
         <v>6.4000000000000001E-2</v>
       </c>
@@ -12700,14 +12710,14 @@
       <c r="M280" s="1">
         <v>0</v>
       </c>
-      <c r="R280" s="1">
+      <c r="R280" s="2">
         <f t="shared" si="3"/>
         <v>0.41999999999999993</v>
       </c>
       <c r="S280" s="1">
         <v>1.97</v>
       </c>
-      <c r="Z280" s="1">
+      <c r="Z280" s="2">
         <f t="shared" si="4"/>
         <v>0.18149999999999999</v>
       </c>
@@ -12740,14 +12750,14 @@
       <c r="M281" s="1">
         <v>5</v>
       </c>
-      <c r="R281" s="1">
+      <c r="R281" s="2">
         <f>S281-1.9</f>
         <v>0.39000000000000012</v>
       </c>
       <c r="S281" s="1">
         <v>2.29</v>
       </c>
-      <c r="Z281" s="1">
+      <c r="Z281" s="2">
         <f>AA281-0.2216</f>
         <v>0.14720000000000003</v>
       </c>
@@ -12780,14 +12790,14 @@
       <c r="M282" s="1">
         <v>5</v>
       </c>
-      <c r="R282" s="1">
+      <c r="R282" s="2">
         <f t="shared" ref="R282:R296" si="5">S282-1.9</f>
         <v>0.18000000000000016</v>
       </c>
       <c r="S282" s="1">
         <v>2.08</v>
       </c>
-      <c r="Z282" s="1">
+      <c r="Z282" s="2">
         <f t="shared" ref="Z282:Z296" si="6">AA282-0.2216</f>
         <v>3.2800000000000024E-2</v>
       </c>
@@ -12820,14 +12830,14 @@
       <c r="M283" s="1">
         <v>5</v>
       </c>
-      <c r="R283" s="1">
+      <c r="R283" s="2">
         <f t="shared" si="5"/>
         <v>0.10000000000000009</v>
       </c>
       <c r="S283" s="1">
         <v>2</v>
       </c>
-      <c r="Z283" s="1">
+      <c r="Z283" s="2">
         <f t="shared" si="6"/>
         <v>2.6700000000000002E-2</v>
       </c>
@@ -12860,14 +12870,14 @@
       <c r="M284" s="1">
         <v>5</v>
       </c>
-      <c r="R284" s="1">
+      <c r="R284" s="2">
         <f t="shared" si="5"/>
         <v>0.52</v>
       </c>
       <c r="S284" s="1">
         <v>2.42</v>
       </c>
-      <c r="Z284" s="1">
+      <c r="Z284" s="2">
         <f t="shared" si="6"/>
         <v>0.21049999999999999</v>
       </c>
@@ -12900,14 +12910,14 @@
       <c r="M285" s="1">
         <v>5</v>
       </c>
-      <c r="R285" s="1">
+      <c r="R285" s="2">
         <f t="shared" si="5"/>
         <v>0.33000000000000007</v>
       </c>
       <c r="S285" s="1">
         <v>2.23</v>
       </c>
-      <c r="Z285" s="1">
+      <c r="Z285" s="2">
         <f t="shared" si="6"/>
         <v>-5.3999999999999965E-2</v>
       </c>
@@ -12940,14 +12950,14 @@
       <c r="M286" s="1">
         <v>5</v>
       </c>
-      <c r="R286" s="1">
+      <c r="R286" s="2">
         <f t="shared" si="5"/>
         <v>0.51000000000000023</v>
       </c>
       <c r="S286" s="1">
         <v>2.41</v>
       </c>
-      <c r="Z286" s="1">
+      <c r="Z286" s="2">
         <f t="shared" si="6"/>
         <v>0.10529999999999998</v>
       </c>
@@ -12980,14 +12990,14 @@
       <c r="M287" s="1">
         <v>5</v>
       </c>
-      <c r="R287" s="1">
+      <c r="R287" s="2">
         <f t="shared" si="5"/>
         <v>0.66999999999999993</v>
       </c>
       <c r="S287" s="1">
         <v>2.57</v>
       </c>
-      <c r="Z287" s="1">
+      <c r="Z287" s="2">
         <f t="shared" si="6"/>
         <v>0.22490000000000002</v>
       </c>
@@ -13020,14 +13030,14 @@
       <c r="M288" s="1">
         <v>5</v>
       </c>
-      <c r="R288" s="1">
+      <c r="R288" s="2">
         <f t="shared" si="5"/>
         <v>0.64000000000000012</v>
       </c>
       <c r="S288" s="1">
         <v>2.54</v>
       </c>
-      <c r="Z288" s="1">
+      <c r="Z288" s="2">
         <f t="shared" si="6"/>
         <v>0.17889999999999998</v>
       </c>
@@ -13060,14 +13070,14 @@
       <c r="M289" s="1">
         <v>5</v>
       </c>
-      <c r="R289" s="1">
+      <c r="R289" s="2">
         <f t="shared" si="5"/>
         <v>0.52</v>
       </c>
       <c r="S289" s="1">
         <v>2.42</v>
       </c>
-      <c r="Z289" s="1">
+      <c r="Z289" s="2">
         <f t="shared" si="6"/>
         <v>0.20699999999999999</v>
       </c>
@@ -13100,14 +13110,14 @@
       <c r="M290" s="1">
         <v>5</v>
       </c>
-      <c r="R290" s="1">
+      <c r="R290" s="2">
         <f t="shared" si="5"/>
         <v>0.49000000000000021</v>
       </c>
       <c r="S290" s="1">
         <v>2.39</v>
       </c>
-      <c r="Z290" s="1">
+      <c r="Z290" s="2">
         <f t="shared" si="6"/>
         <v>0.20040000000000005</v>
       </c>
@@ -13140,14 +13150,14 @@
       <c r="M291" s="1">
         <v>5</v>
       </c>
-      <c r="R291" s="1">
+      <c r="R291" s="2">
         <f t="shared" si="5"/>
         <v>0.62999999999999989</v>
       </c>
       <c r="S291" s="1">
         <v>2.5299999999999998</v>
       </c>
-      <c r="Z291" s="1">
+      <c r="Z291" s="2">
         <f t="shared" si="6"/>
         <v>0.20819999999999997</v>
       </c>
@@ -13180,14 +13190,14 @@
       <c r="M292" s="1">
         <v>5</v>
       </c>
-      <c r="R292" s="1">
+      <c r="R292" s="2">
         <f t="shared" si="5"/>
         <v>0.25</v>
       </c>
       <c r="S292" s="1">
         <v>2.15</v>
       </c>
-      <c r="Z292" s="1">
+      <c r="Z292" s="2">
         <f t="shared" si="6"/>
         <v>0.14959999999999998</v>
       </c>
@@ -13220,14 +13230,14 @@
       <c r="M293" s="1">
         <v>5</v>
       </c>
-      <c r="R293" s="1">
+      <c r="R293" s="2">
         <f t="shared" si="5"/>
         <v>0.62000000000000011</v>
       </c>
       <c r="S293" s="1">
         <v>2.52</v>
       </c>
-      <c r="Z293" s="1">
+      <c r="Z293" s="2">
         <f t="shared" si="6"/>
         <v>0.20730000000000001</v>
       </c>
@@ -13260,14 +13270,14 @@
       <c r="M294" s="1">
         <v>5</v>
       </c>
-      <c r="R294" s="1">
+      <c r="R294" s="2">
         <f t="shared" si="5"/>
         <v>0.62999999999999989</v>
       </c>
       <c r="S294" s="1">
         <v>2.5299999999999998</v>
       </c>
-      <c r="Z294" s="1">
+      <c r="Z294" s="2">
         <f t="shared" si="6"/>
         <v>0.2392</v>
       </c>
@@ -13300,14 +13310,14 @@
       <c r="M295" s="1">
         <v>5</v>
       </c>
-      <c r="R295" s="1">
+      <c r="R295" s="2">
         <f t="shared" si="5"/>
         <v>0.70000000000000018</v>
       </c>
       <c r="S295" s="1">
         <v>2.6</v>
       </c>
-      <c r="Z295" s="1">
+      <c r="Z295" s="2">
         <f t="shared" si="6"/>
         <v>9.080000000000002E-2</v>
       </c>
@@ -13340,14 +13350,14 @@
       <c r="M296" s="1">
         <v>5</v>
       </c>
-      <c r="R296" s="1">
+      <c r="R296" s="2">
         <f t="shared" si="5"/>
         <v>0.37999999999999989</v>
       </c>
       <c r="S296" s="1">
         <v>2.2799999999999998</v>
       </c>
-      <c r="Z296" s="1">
+      <c r="Z296" s="2">
         <f t="shared" si="6"/>
         <v>0.18139999999999998</v>
       </c>
@@ -13380,14 +13390,14 @@
       <c r="M297" s="1">
         <v>10</v>
       </c>
-      <c r="R297" s="1">
+      <c r="R297" s="2">
         <f>S297-2.26</f>
         <v>0.46000000000000041</v>
       </c>
       <c r="S297" s="1">
         <v>2.72</v>
       </c>
-      <c r="Z297" s="1">
+      <c r="Z297" s="2">
         <f>AA297-0.33</f>
         <v>0.13250000000000001</v>
       </c>
@@ -13420,14 +13430,14 @@
       <c r="M298" s="1">
         <v>10</v>
       </c>
-      <c r="R298" s="1">
+      <c r="R298" s="2">
         <f t="shared" ref="R298:R312" si="7">S298-2.26</f>
         <v>0.32000000000000028</v>
       </c>
       <c r="S298" s="1">
         <v>2.58</v>
       </c>
-      <c r="Z298" s="1">
+      <c r="Z298" s="2">
         <f>AA298-0.33</f>
         <v>4.8399999999999999E-2</v>
       </c>
@@ -13460,14 +13470,14 @@
       <c r="M299" s="1">
         <v>10</v>
       </c>
-      <c r="R299" s="1">
+      <c r="R299" s="2">
         <f t="shared" si="7"/>
         <v>0.15000000000000036</v>
       </c>
       <c r="S299" s="1">
         <v>2.41</v>
       </c>
-      <c r="Z299" s="1">
+      <c r="Z299" s="2">
         <f>AA299-0.33</f>
         <v>3.4999999999999976E-2</v>
       </c>
@@ -13500,14 +13510,14 @@
       <c r="M300" s="1">
         <v>10</v>
       </c>
-      <c r="R300" s="1">
+      <c r="R300" s="2">
         <f t="shared" si="7"/>
         <v>0.53000000000000025</v>
       </c>
       <c r="S300" s="1">
         <v>2.79</v>
       </c>
-      <c r="Z300" s="1">
+      <c r="Z300" s="2">
         <f t="shared" ref="Z300:Z312" si="8">AA300-0.33</f>
         <v>0.2152</v>
       </c>
@@ -13540,14 +13550,14 @@
       <c r="M301" s="1">
         <v>10</v>
       </c>
-      <c r="R301" s="1">
+      <c r="R301" s="2">
         <f t="shared" si="7"/>
         <v>0.38000000000000034</v>
       </c>
       <c r="S301" s="1">
         <v>2.64</v>
       </c>
-      <c r="Z301" s="1">
+      <c r="Z301" s="2">
         <f t="shared" si="8"/>
         <v>-3.3999999999999975E-2</v>
       </c>
@@ -13580,14 +13590,14 @@
       <c r="M302" s="1">
         <v>10</v>
       </c>
-      <c r="R302" s="1">
+      <c r="R302" s="2">
         <f t="shared" si="7"/>
         <v>0.48000000000000043</v>
       </c>
       <c r="S302" s="1">
         <v>2.74</v>
       </c>
-      <c r="Z302" s="1">
+      <c r="Z302" s="2">
         <f t="shared" si="8"/>
         <v>0.10609999999999997</v>
       </c>
@@ -13620,14 +13630,14 @@
       <c r="M303" s="1">
         <v>10</v>
       </c>
-      <c r="R303" s="1">
+      <c r="R303" s="2">
         <f t="shared" si="7"/>
         <v>0.67000000000000037</v>
       </c>
       <c r="S303" s="1">
         <v>2.93</v>
       </c>
-      <c r="Z303" s="1">
+      <c r="Z303" s="2">
         <f t="shared" si="8"/>
         <v>0.22189999999999993</v>
       </c>
@@ -13660,14 +13670,14 @@
       <c r="M304" s="1">
         <v>10</v>
       </c>
-      <c r="R304" s="1">
+      <c r="R304" s="2">
         <f t="shared" si="7"/>
         <v>0.62000000000000011</v>
       </c>
       <c r="S304" s="1">
         <v>2.88</v>
       </c>
-      <c r="Z304" s="1">
+      <c r="Z304" s="2">
         <f t="shared" si="8"/>
         <v>0.17740000000000006</v>
       </c>
@@ -13700,14 +13710,14 @@
       <c r="M305" s="1">
         <v>10</v>
       </c>
-      <c r="R305" s="1">
+      <c r="R305" s="2">
         <f t="shared" si="7"/>
         <v>0.58000000000000007</v>
       </c>
       <c r="S305" s="1">
         <v>2.84</v>
       </c>
-      <c r="Z305" s="1">
+      <c r="Z305" s="2">
         <f t="shared" si="8"/>
         <v>0.19039999999999996</v>
       </c>
@@ -13740,14 +13750,14 @@
       <c r="M306" s="1">
         <v>10</v>
       </c>
-      <c r="R306" s="1">
+      <c r="R306" s="2">
         <f t="shared" si="7"/>
         <v>0.55000000000000027</v>
       </c>
       <c r="S306" s="1">
         <v>2.81</v>
       </c>
-      <c r="Z306" s="1">
+      <c r="Z306" s="2">
         <f t="shared" si="8"/>
         <v>0.18869999999999992</v>
       </c>
@@ -13780,14 +13790,14 @@
       <c r="M307" s="1">
         <v>10</v>
       </c>
-      <c r="R307" s="1">
+      <c r="R307" s="2">
         <f t="shared" si="7"/>
         <v>0.64000000000000012</v>
       </c>
       <c r="S307" s="1">
         <v>2.9</v>
       </c>
-      <c r="Z307" s="1">
+      <c r="Z307" s="2">
         <f t="shared" si="8"/>
         <v>0.20359999999999995</v>
       </c>
@@ -13820,14 +13830,14 @@
       <c r="M308" s="1">
         <v>10</v>
       </c>
-      <c r="R308" s="1">
+      <c r="R308" s="2">
         <f t="shared" si="7"/>
         <v>0.28000000000000025</v>
       </c>
       <c r="S308" s="1">
         <v>2.54</v>
       </c>
-      <c r="Z308" s="1">
+      <c r="Z308" s="2">
         <f t="shared" si="8"/>
         <v>0.13109999999999999</v>
       </c>
@@ -13860,14 +13870,14 @@
       <c r="M309" s="1">
         <v>10</v>
       </c>
-      <c r="R309" s="1">
+      <c r="R309" s="2">
         <f t="shared" si="7"/>
         <v>0.62000000000000011</v>
       </c>
       <c r="S309" s="1">
         <v>2.88</v>
       </c>
-      <c r="Z309" s="1">
+      <c r="Z309" s="2">
         <f t="shared" si="8"/>
         <v>0.21299999999999991</v>
       </c>
@@ -13900,14 +13910,14 @@
       <c r="M310" s="1">
         <v>10</v>
       </c>
-      <c r="R310" s="1">
+      <c r="R310" s="2">
         <f t="shared" si="7"/>
         <v>0.61000000000000032</v>
       </c>
       <c r="S310" s="1">
         <v>2.87</v>
       </c>
-      <c r="Z310" s="1">
+      <c r="Z310" s="2">
         <f t="shared" si="8"/>
         <v>0.21789999999999993</v>
       </c>
@@ -13940,14 +13950,14 @@
       <c r="M311" s="1">
         <v>10</v>
       </c>
-      <c r="R311" s="1">
+      <c r="R311" s="2">
         <f t="shared" si="7"/>
         <v>0.71000000000000041</v>
       </c>
       <c r="S311" s="1">
         <v>2.97</v>
       </c>
-      <c r="Z311" s="1">
+      <c r="Z311" s="2">
         <f t="shared" si="8"/>
         <v>9.7599999999999965E-2</v>
       </c>
@@ -13980,14 +13990,14 @@
       <c r="M312" s="1">
         <v>10</v>
       </c>
-      <c r="R312" s="1">
+      <c r="R312" s="2">
         <f t="shared" si="7"/>
         <v>0.38000000000000034</v>
       </c>
       <c r="S312" s="1">
         <v>2.64</v>
       </c>
-      <c r="Z312" s="1">
+      <c r="Z312" s="2">
         <f t="shared" si="8"/>
         <v>0.15649999999999997</v>
       </c>
@@ -14020,14 +14030,14 @@
       <c r="M313" s="1">
         <v>15</v>
       </c>
-      <c r="R313" s="1">
+      <c r="R313" s="2">
         <f>S313-2.62</f>
         <v>0.54999999999999982</v>
       </c>
       <c r="S313" s="1">
         <v>3.17</v>
       </c>
-      <c r="Z313" s="1">
+      <c r="Z313" s="2">
         <f>AA313-0.4531</f>
         <v>0.11300000000000004</v>
       </c>
@@ -14060,14 +14070,14 @@
       <c r="M314" s="1">
         <v>15</v>
       </c>
-      <c r="R314" s="1">
+      <c r="R314" s="2">
         <f t="shared" ref="R314:R328" si="9">S314-2.62</f>
         <v>0.35000000000000009</v>
       </c>
       <c r="S314" s="1">
         <v>2.97</v>
       </c>
-      <c r="Z314" s="1">
+      <c r="Z314" s="2">
         <f t="shared" ref="Z314" si="10">AA314-0.4531</f>
         <v>6.750000000000006E-2</v>
       </c>
@@ -14100,14 +14110,14 @@
       <c r="M315" s="1">
         <v>15</v>
       </c>
-      <c r="R315" s="1">
+      <c r="R315" s="2">
         <f t="shared" si="9"/>
         <v>0.19999999999999973</v>
       </c>
       <c r="S315" s="1">
         <v>2.82</v>
       </c>
-      <c r="Z315" s="1">
+      <c r="Z315" s="2">
         <f t="shared" ref="Z315" si="11">AA315-0.4531</f>
         <v>4.5099999999999973E-2</v>
       </c>
@@ -14140,14 +14150,14 @@
       <c r="M316" s="1">
         <v>15</v>
       </c>
-      <c r="R316" s="1">
+      <c r="R316" s="2">
         <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
       <c r="S316" s="1">
         <v>3.12</v>
       </c>
-      <c r="Z316" s="1">
+      <c r="Z316" s="2">
         <f t="shared" ref="Z316" si="12">AA316-0.4531</f>
         <v>0.17829999999999996</v>
       </c>
@@ -14180,14 +14190,14 @@
       <c r="M317" s="1">
         <v>15</v>
       </c>
-      <c r="R317" s="1">
+      <c r="R317" s="2">
         <f t="shared" si="9"/>
         <v>0.44999999999999973</v>
       </c>
       <c r="S317" s="1">
         <v>3.07</v>
       </c>
-      <c r="Z317" s="1">
+      <c r="Z317" s="2">
         <f t="shared" ref="Z317" si="13">AA317-0.4531</f>
         <v>-1.1399999999999966E-2</v>
       </c>
@@ -14220,14 +14230,14 @@
       <c r="M318" s="1">
         <v>15</v>
       </c>
-      <c r="R318" s="1">
+      <c r="R318" s="2">
         <f t="shared" si="9"/>
         <v>0.42999999999999972</v>
       </c>
       <c r="S318" s="1">
         <v>3.05</v>
       </c>
-      <c r="Z318" s="1">
+      <c r="Z318" s="2">
         <f t="shared" ref="Z318" si="14">AA318-0.4531</f>
         <v>9.7299999999999998E-2</v>
       </c>
@@ -14260,14 +14270,14 @@
       <c r="M319" s="1">
         <v>15</v>
       </c>
-      <c r="R319" s="1">
+      <c r="R319" s="2">
         <f t="shared" si="9"/>
         <v>0.62999999999999989</v>
       </c>
       <c r="S319" s="1">
         <v>3.25</v>
       </c>
-      <c r="Z319" s="1">
+      <c r="Z319" s="2">
         <f t="shared" ref="Z319" si="15">AA319-0.4531</f>
         <v>0.18209999999999998</v>
       </c>
@@ -14300,14 +14310,14 @@
       <c r="M320" s="1">
         <v>15</v>
       </c>
-      <c r="R320" s="1">
+      <c r="R320" s="2">
         <f t="shared" si="9"/>
         <v>0.54999999999999982</v>
       </c>
       <c r="S320" s="1">
         <v>3.17</v>
       </c>
-      <c r="Z320" s="1">
+      <c r="Z320" s="2">
         <f t="shared" ref="Z320" si="16">AA320-0.4531</f>
         <v>0.15160000000000001</v>
       </c>
@@ -14340,14 +14350,14 @@
       <c r="M321" s="1">
         <v>15</v>
       </c>
-      <c r="R321" s="1">
+      <c r="R321" s="2">
         <f t="shared" si="9"/>
         <v>0.58999999999999986</v>
       </c>
       <c r="S321" s="1">
         <v>3.21</v>
       </c>
-      <c r="Z321" s="1">
+      <c r="Z321" s="2">
         <f t="shared" ref="Z321" si="17">AA321-0.4531</f>
         <v>0.11890000000000006</v>
       </c>
@@ -14380,14 +14390,14 @@
       <c r="M322" s="1">
         <v>15</v>
       </c>
-      <c r="R322" s="1">
+      <c r="R322" s="2">
         <f t="shared" si="9"/>
         <v>0.58000000000000007</v>
       </c>
       <c r="S322" s="1">
         <v>3.2</v>
       </c>
-      <c r="Z322" s="1">
+      <c r="Z322" s="2">
         <f t="shared" ref="Z322" si="18">AA322-0.4531</f>
         <v>0.11459999999999998</v>
       </c>
@@ -14420,14 +14430,14 @@
       <c r="M323" s="1">
         <v>15</v>
       </c>
-      <c r="R323" s="1">
+      <c r="R323" s="2">
         <f t="shared" si="9"/>
         <v>0.62999999999999989</v>
       </c>
       <c r="S323" s="1">
         <v>3.25</v>
       </c>
-      <c r="Z323" s="1">
+      <c r="Z323" s="2">
         <f t="shared" ref="Z323" si="19">AA323-0.4531</f>
         <v>0.14299999999999996</v>
       </c>
@@ -14460,14 +14470,14 @@
       <c r="M324" s="1">
         <v>15</v>
       </c>
-      <c r="R324" s="1">
+      <c r="R324" s="2">
         <f t="shared" si="9"/>
         <v>0.25999999999999979</v>
       </c>
       <c r="S324" s="1">
         <v>2.88</v>
       </c>
-      <c r="Z324" s="1">
+      <c r="Z324" s="2">
         <f t="shared" ref="Z324" si="20">AA324-0.4531</f>
         <v>8.4199999999999997E-2</v>
       </c>
@@ -14500,14 +14510,14 @@
       <c r="M325" s="1">
         <v>15</v>
       </c>
-      <c r="R325" s="1">
+      <c r="R325" s="2">
         <f t="shared" si="9"/>
         <v>0.58000000000000007</v>
       </c>
       <c r="S325" s="1">
         <v>3.2</v>
       </c>
-      <c r="Z325" s="1">
+      <c r="Z325" s="2">
         <f t="shared" ref="Z325" si="21">AA325-0.4531</f>
         <v>0.16820000000000007</v>
       </c>
@@ -14540,14 +14550,14 @@
       <c r="M326" s="1">
         <v>15</v>
       </c>
-      <c r="R326" s="1">
+      <c r="R326" s="2">
         <f t="shared" si="9"/>
         <v>0.58000000000000007</v>
       </c>
       <c r="S326" s="1">
         <v>3.2</v>
       </c>
-      <c r="Z326" s="1">
+      <c r="Z326" s="2">
         <f t="shared" ref="Z326" si="22">AA326-0.4531</f>
         <v>0.16499999999999998</v>
       </c>
@@ -14580,14 +14590,14 @@
       <c r="M327" s="1">
         <v>15</v>
       </c>
-      <c r="R327" s="1">
+      <c r="R327" s="2">
         <f t="shared" si="9"/>
         <v>0.71999999999999975</v>
       </c>
       <c r="S327" s="1">
         <v>3.34</v>
       </c>
-      <c r="Z327" s="1">
+      <c r="Z327" s="2">
         <f t="shared" ref="Z327" si="23">AA327-0.4531</f>
         <v>6.5399999999999958E-2</v>
       </c>
@@ -14620,14 +14630,14 @@
       <c r="M328" s="1">
         <v>15</v>
       </c>
-      <c r="R328" s="1">
+      <c r="R328" s="2">
         <f t="shared" si="9"/>
         <v>0.39999999999999991</v>
       </c>
       <c r="S328" s="1">
         <v>3.02</v>
       </c>
-      <c r="Z328" s="1">
+      <c r="Z328" s="2">
         <f t="shared" ref="Z328" si="24">AA328-0.4531</f>
         <v>0.11049999999999999</v>
       </c>
@@ -14660,14 +14670,14 @@
       <c r="M329" s="1">
         <v>20</v>
       </c>
-      <c r="R329" s="1">
+      <c r="R329" s="2">
         <f>S329-2.97</f>
         <v>0.60999999999999988</v>
       </c>
       <c r="S329" s="1">
         <v>3.58</v>
       </c>
-      <c r="Z329" s="1">
+      <c r="Z329" s="2">
         <f>AA329-0.5595</f>
         <v>7.569999999999999E-2</v>
       </c>
@@ -14700,14 +14710,14 @@
       <c r="M330" s="1">
         <v>20</v>
       </c>
-      <c r="R330" s="1">
+      <c r="R330" s="2">
         <f t="shared" ref="R330:R344" si="25">S330-2.97</f>
         <v>0.23999999999999977</v>
       </c>
       <c r="S330" s="1">
         <v>3.21</v>
       </c>
-      <c r="Z330" s="1">
+      <c r="Z330" s="2">
         <f t="shared" ref="Z330" si="26">AA330-0.5595</f>
         <v>4.930000000000001E-2</v>
       </c>
@@ -14740,14 +14750,14 @@
       <c r="M331" s="1">
         <v>20</v>
       </c>
-      <c r="R331" s="1">
+      <c r="R331" s="2">
         <f t="shared" si="25"/>
         <v>0.23999999999999977</v>
       </c>
       <c r="S331" s="1">
         <v>3.21</v>
       </c>
-      <c r="Z331" s="1">
+      <c r="Z331" s="2">
         <f t="shared" ref="Z331" si="27">AA331-0.5595</f>
         <v>6.1499999999999999E-2</v>
       </c>
@@ -14780,14 +14790,14 @@
       <c r="M332" s="1">
         <v>20</v>
       </c>
-      <c r="R332" s="1">
+      <c r="R332" s="2">
         <f t="shared" si="25"/>
         <v>0.45999999999999996</v>
       </c>
       <c r="S332" s="1">
         <v>3.43</v>
       </c>
-      <c r="Z332" s="1">
+      <c r="Z332" s="2">
         <f t="shared" ref="Z332" si="28">AA332-0.5595</f>
         <v>0.12239999999999995</v>
       </c>
@@ -14820,14 +14830,14 @@
       <c r="M333" s="1">
         <v>20</v>
       </c>
-      <c r="R333" s="1">
+      <c r="R333" s="2">
         <f t="shared" si="25"/>
         <v>0.48</v>
       </c>
       <c r="S333" s="1">
         <v>3.45</v>
       </c>
-      <c r="Z333" s="1">
+      <c r="Z333" s="2">
         <f t="shared" ref="Z333" si="29">AA333-0.5595</f>
         <v>2.8000000000000247E-3</v>
       </c>
@@ -14860,14 +14870,14 @@
       <c r="M334" s="1">
         <v>20</v>
       </c>
-      <c r="R334" s="1">
+      <c r="R334" s="2">
         <f t="shared" si="25"/>
         <v>0.35999999999999988</v>
       </c>
       <c r="S334" s="1">
         <v>3.33</v>
       </c>
-      <c r="Z334" s="1">
+      <c r="Z334" s="2">
         <f t="shared" ref="Z334" si="30">AA334-0.5595</f>
         <v>7.7200000000000046E-2</v>
       </c>
@@ -14900,14 +14910,14 @@
       <c r="M335" s="1">
         <v>20</v>
       </c>
-      <c r="R335" s="1">
+      <c r="R335" s="2">
         <f t="shared" si="25"/>
         <v>0.60999999999999988</v>
       </c>
       <c r="S335" s="1">
         <v>3.58</v>
       </c>
-      <c r="Z335" s="1">
+      <c r="Z335" s="2">
         <f t="shared" ref="Z335" si="31">AA335-0.5595</f>
         <v>0.12080000000000002</v>
       </c>
@@ -14940,14 +14950,14 @@
       <c r="M336" s="1">
         <v>20</v>
       </c>
-      <c r="R336" s="1">
+      <c r="R336" s="2">
         <f t="shared" si="25"/>
         <v>0.48</v>
       </c>
       <c r="S336" s="1">
         <v>3.45</v>
       </c>
-      <c r="Z336" s="1">
+      <c r="Z336" s="2">
         <f t="shared" ref="Z336" si="32">AA336-0.5595</f>
         <v>0.10980000000000012</v>
       </c>
@@ -14980,14 +14990,14 @@
       <c r="M337" s="1">
         <v>20</v>
       </c>
-      <c r="R337" s="1">
+      <c r="R337" s="2">
         <f t="shared" si="25"/>
         <v>0.56999999999999984</v>
       </c>
       <c r="S337" s="1">
         <v>3.54</v>
       </c>
-      <c r="Z337" s="1">
+      <c r="Z337" s="2">
         <f t="shared" ref="Z337" si="33">AA337-0.5595</f>
         <v>5.8099999999999929E-2</v>
       </c>
@@ -15020,14 +15030,14 @@
       <c r="M338" s="1">
         <v>20</v>
       </c>
-      <c r="R338" s="1">
+      <c r="R338" s="2">
         <f t="shared" si="25"/>
         <v>0.54999999999999982</v>
       </c>
       <c r="S338" s="1">
         <v>3.52</v>
       </c>
-      <c r="Z338" s="1">
+      <c r="Z338" s="2">
         <f t="shared" ref="Z338" si="34">AA338-0.5595</f>
         <v>5.1100000000000034E-2</v>
       </c>
@@ -15060,14 +15070,14 @@
       <c r="M339" s="1">
         <v>20</v>
       </c>
-      <c r="R339" s="1">
+      <c r="R339" s="2">
         <f t="shared" si="25"/>
         <v>0.57999999999999963</v>
       </c>
       <c r="S339" s="1">
         <v>3.55</v>
       </c>
-      <c r="Z339" s="1">
+      <c r="Z339" s="2">
         <f t="shared" ref="Z339" si="35">AA339-0.5595</f>
         <v>9.0300000000000047E-2</v>
       </c>
@@ -15100,14 +15110,14 @@
       <c r="M340" s="1">
         <v>20</v>
       </c>
-      <c r="R340" s="1">
+      <c r="R340" s="2">
         <f t="shared" si="25"/>
         <v>0.28999999999999959</v>
       </c>
       <c r="S340" s="1">
         <v>3.26</v>
       </c>
-      <c r="Z340" s="1">
+      <c r="Z340" s="2">
         <f t="shared" ref="Z340" si="36">AA340-0.5595</f>
         <v>6.4100000000000046E-2</v>
       </c>
@@ -15140,14 +15150,14 @@
       <c r="M341" s="1">
         <v>20</v>
       </c>
-      <c r="R341" s="1">
+      <c r="R341" s="2">
         <f t="shared" si="25"/>
         <v>0.53999999999999959</v>
       </c>
       <c r="S341" s="1">
         <v>3.51</v>
       </c>
-      <c r="Z341" s="1">
+      <c r="Z341" s="2">
         <f t="shared" ref="Z341" si="37">AA341-0.5595</f>
         <v>0.1070000000000001</v>
       </c>
@@ -15180,14 +15190,14 @@
       <c r="M342" s="1">
         <v>20</v>
       </c>
-      <c r="R342" s="1">
+      <c r="R342" s="2">
         <f t="shared" si="25"/>
         <v>0.53999999999999959</v>
       </c>
       <c r="S342" s="1">
         <v>3.51</v>
       </c>
-      <c r="Z342" s="1">
+      <c r="Z342" s="2">
         <f t="shared" ref="Z342" si="38">AA342-0.5595</f>
         <v>9.5700000000000007E-2</v>
       </c>
@@ -15220,14 +15230,14 @@
       <c r="M343" s="1">
         <v>20</v>
       </c>
-      <c r="R343" s="1">
+      <c r="R343" s="2">
         <f t="shared" si="25"/>
         <v>0.69</v>
       </c>
       <c r="S343" s="1">
         <v>3.66</v>
       </c>
-      <c r="Z343" s="1">
+      <c r="Z343" s="2">
         <f t="shared" ref="Z343" si="39">AA343-0.5595</f>
         <v>4.6300000000000008E-2</v>
       </c>
@@ -15260,14 +15270,14 @@
       <c r="M344" s="1">
         <v>20</v>
       </c>
-      <c r="R344" s="1">
+      <c r="R344" s="2">
         <f t="shared" si="25"/>
         <v>0.42999999999999972</v>
       </c>
       <c r="S344" s="1">
         <v>3.4</v>
       </c>
-      <c r="Z344" s="1">
+      <c r="Z344" s="2">
         <f t="shared" ref="Z344" si="40">AA344-0.5595</f>
         <v>6.4400000000000013E-2</v>
       </c>
@@ -15300,14 +15310,14 @@
       <c r="M345" s="1">
         <v>25</v>
       </c>
-      <c r="R345" s="1">
+      <c r="R345" s="2">
         <f>S345-3.31</f>
         <v>0.58999999999999986</v>
       </c>
       <c r="S345" s="1">
         <v>3.9</v>
       </c>
-      <c r="Z345" s="1">
+      <c r="Z345" s="2">
         <f>AA345-0.6473</f>
         <v>4.1000000000000036E-2</v>
       </c>
@@ -15340,14 +15350,14 @@
       <c r="M346" s="1">
         <v>25</v>
       </c>
-      <c r="R346" s="1">
+      <c r="R346" s="2">
         <f t="shared" ref="R346:R360" si="41">S346-3.31</f>
         <v>6.999999999999984E-2</v>
       </c>
       <c r="S346" s="1">
         <v>3.38</v>
       </c>
-      <c r="Z346" s="1">
+      <c r="Z346" s="2">
         <f t="shared" ref="Z346" si="42">AA346-0.6473</f>
         <v>1.8800000000000039E-2</v>
       </c>
@@ -15380,14 +15390,14 @@
       <c r="M347" s="1">
         <v>25</v>
       </c>
-      <c r="R347" s="1">
+      <c r="R347" s="2">
         <f t="shared" si="41"/>
         <v>0.27</v>
       </c>
       <c r="S347" s="1">
         <v>3.58</v>
       </c>
-      <c r="Z347" s="1">
+      <c r="Z347" s="2">
         <f t="shared" ref="Z347" si="43">AA347-0.6473</f>
         <v>5.3200000000000025E-2</v>
       </c>
@@ -15420,14 +15430,14 @@
       <c r="M348" s="1">
         <v>25</v>
       </c>
-      <c r="R348" s="1">
+      <c r="R348" s="2">
         <f t="shared" si="41"/>
         <v>0.41000000000000014</v>
       </c>
       <c r="S348" s="1">
         <v>3.72</v>
       </c>
-      <c r="Z348" s="1">
+      <c r="Z348" s="2">
         <f t="shared" ref="Z348" si="44">AA348-0.6473</f>
         <v>7.46E-2</v>
       </c>
@@ -15460,14 +15470,14 @@
       <c r="M349" s="1">
         <v>25</v>
       </c>
-      <c r="R349" s="1">
+      <c r="R349" s="2">
         <f t="shared" si="41"/>
         <v>0.48</v>
       </c>
       <c r="S349" s="1">
         <v>3.79</v>
       </c>
-      <c r="Z349" s="1">
+      <c r="Z349" s="2">
         <f t="shared" ref="Z349" si="45">AA349-0.6473</f>
         <v>-1.1399999999999966E-2</v>
       </c>
@@ -15500,14 +15510,14 @@
       <c r="M350" s="1">
         <v>25</v>
       </c>
-      <c r="R350" s="1">
+      <c r="R350" s="2">
         <f t="shared" si="41"/>
         <v>0.29999999999999982</v>
       </c>
       <c r="S350" s="1">
         <v>3.61</v>
       </c>
-      <c r="Z350" s="1">
+      <c r="Z350" s="2">
         <f t="shared" ref="Z350" si="46">AA350-0.6473</f>
         <v>4.8399999999999999E-2</v>
       </c>
@@ -15540,14 +15550,14 @@
       <c r="M351" s="1">
         <v>25</v>
       </c>
-      <c r="R351" s="1">
+      <c r="R351" s="2">
         <f t="shared" si="41"/>
         <v>0.56000000000000005</v>
       </c>
       <c r="S351" s="1">
         <v>3.87</v>
       </c>
-      <c r="Z351" s="1">
+      <c r="Z351" s="2">
         <f t="shared" ref="Z351" si="47">AA351-0.6473</f>
         <v>6.140000000000001E-2</v>
       </c>
@@ -15580,14 +15590,14 @@
       <c r="M352" s="1">
         <v>25</v>
       </c>
-      <c r="R352" s="1">
+      <c r="R352" s="2">
         <f t="shared" si="41"/>
         <v>0.39999999999999991</v>
       </c>
       <c r="S352" s="1">
         <v>3.71</v>
       </c>
-      <c r="Z352" s="1">
+      <c r="Z352" s="2">
         <f t="shared" ref="Z352" si="48">AA352-0.6473</f>
         <v>6.5200000000000036E-2</v>
       </c>
@@ -15620,14 +15630,14 @@
       <c r="M353" s="1">
         <v>25</v>
       </c>
-      <c r="R353" s="1">
+      <c r="R353" s="2">
         <f t="shared" si="41"/>
         <v>0.48999999999999977</v>
       </c>
       <c r="S353" s="1">
         <v>3.8</v>
       </c>
-      <c r="Z353" s="1">
+      <c r="Z353" s="2">
         <f t="shared" ref="Z353" si="49">AA353-0.6473</f>
         <v>1.0099999999999998E-2</v>
       </c>
@@ -15660,14 +15670,14 @@
       <c r="M354" s="1">
         <v>25</v>
       </c>
-      <c r="R354" s="1">
+      <c r="R354" s="2">
         <f t="shared" si="41"/>
         <v>0.46999999999999975</v>
       </c>
       <c r="S354" s="1">
         <v>3.78</v>
       </c>
-      <c r="Z354" s="1">
+      <c r="Z354" s="2">
         <f t="shared" ref="Z354" si="50">AA354-0.6473</f>
         <v>1.1999999999999789E-3</v>
       </c>
@@ -15700,14 +15710,14 @@
       <c r="M355" s="1">
         <v>25</v>
       </c>
-      <c r="R355" s="1">
+      <c r="R355" s="2">
         <f t="shared" si="41"/>
         <v>0.50999999999999979</v>
       </c>
       <c r="S355" s="1">
         <v>3.82</v>
       </c>
-      <c r="Z355" s="1">
+      <c r="Z355" s="2">
         <f t="shared" ref="Z355" si="51">AA355-0.6473</f>
         <v>4.0899999999999936E-2</v>
       </c>
@@ -15740,14 +15750,14 @@
       <c r="M356" s="1">
         <v>25</v>
       </c>
-      <c r="R356" s="1">
+      <c r="R356" s="2">
         <f t="shared" si="41"/>
         <v>0.29000000000000004</v>
       </c>
       <c r="S356" s="1">
         <v>3.6</v>
       </c>
-      <c r="Z356" s="1">
+      <c r="Z356" s="2">
         <f t="shared" ref="Z356" si="52">AA356-0.6473</f>
         <v>3.4299999999999997E-2</v>
       </c>
@@ -15780,14 +15790,14 @@
       <c r="M357" s="1">
         <v>25</v>
       </c>
-      <c r="R357" s="1">
+      <c r="R357" s="2">
         <f t="shared" si="41"/>
         <v>0.46999999999999975</v>
       </c>
       <c r="S357" s="1">
         <v>3.78</v>
       </c>
-      <c r="Z357" s="1">
+      <c r="Z357" s="2">
         <f t="shared" ref="Z357" si="53">AA357-0.6473</f>
         <v>4.9399999999999999E-2</v>
       </c>
@@ -15820,14 +15830,14 @@
       <c r="M358" s="1">
         <v>25</v>
       </c>
-      <c r="R358" s="1">
+      <c r="R358" s="2">
         <f t="shared" si="41"/>
         <v>0.48</v>
       </c>
       <c r="S358" s="1">
         <v>3.79</v>
       </c>
-      <c r="Z358" s="1">
+      <c r="Z358" s="2">
         <f t="shared" ref="Z358" si="54">AA358-0.6473</f>
         <v>3.9100000000000024E-2</v>
       </c>
@@ -15860,14 +15870,14 @@
       <c r="M359" s="1">
         <v>25</v>
       </c>
-      <c r="R359" s="1">
+      <c r="R359" s="2">
         <f t="shared" si="41"/>
         <v>0.60999999999999988</v>
       </c>
       <c r="S359" s="1">
         <v>3.92</v>
       </c>
-      <c r="Z359" s="1">
+      <c r="Z359" s="2">
         <f t="shared" ref="Z359" si="55">AA359-0.6473</f>
         <v>1.6600000000000059E-2</v>
       </c>
@@ -15900,14 +15910,14 @@
       <c r="M360" s="1">
         <v>25</v>
       </c>
-      <c r="R360" s="1">
+      <c r="R360" s="2">
         <f t="shared" si="41"/>
         <v>0.41999999999999993</v>
       </c>
       <c r="S360" s="1">
         <v>3.73</v>
       </c>
-      <c r="Z360" s="1">
+      <c r="Z360" s="2">
         <f t="shared" ref="Z360" si="56">AA360-0.6473</f>
         <v>1.7900000000000027E-2</v>
       </c>
@@ -15940,14 +15950,14 @@
       <c r="M361" s="1">
         <v>30</v>
       </c>
-      <c r="R361" s="1">
+      <c r="R361" s="2">
         <f>S361-3.64</f>
         <v>0.48</v>
       </c>
       <c r="S361" s="1">
         <v>4.12</v>
       </c>
-      <c r="Z361" s="1">
+      <c r="Z361" s="2">
         <f>AA361-0.7052</f>
         <v>2.4999999999999911E-2</v>
       </c>
@@ -15980,14 +15990,14 @@
       <c r="M362" s="1">
         <v>30</v>
       </c>
-      <c r="R362" s="1">
+      <c r="R362" s="2">
         <f t="shared" ref="R362:R376" si="57">S362-3.64</f>
         <v>-0.14999999999999991</v>
       </c>
       <c r="S362" s="1">
         <v>3.49</v>
       </c>
-      <c r="Z362" s="1">
+      <c r="Z362" s="2">
         <f t="shared" ref="Z362" si="58">AA362-0.7052</f>
         <v>-2.4600000000000066E-2</v>
       </c>
@@ -16020,14 +16030,14 @@
       <c r="M363" s="1">
         <v>30</v>
       </c>
-      <c r="R363" s="1">
+      <c r="R363" s="2">
         <f t="shared" si="57"/>
         <v>0.29000000000000004</v>
       </c>
       <c r="S363" s="1">
         <v>3.93</v>
       </c>
-      <c r="Z363" s="1">
+      <c r="Z363" s="2">
         <f t="shared" ref="Z363" si="59">AA363-0.7052</f>
         <v>3.5399999999999987E-2</v>
       </c>
@@ -16060,14 +16070,14 @@
       <c r="M364" s="1">
         <v>30</v>
       </c>
-      <c r="R364" s="1">
+      <c r="R364" s="2">
         <f t="shared" si="57"/>
         <v>0.35000000000000009</v>
       </c>
       <c r="S364" s="1">
         <v>3.99</v>
       </c>
-      <c r="Z364" s="1">
+      <c r="Z364" s="2">
         <f t="shared" ref="Z364" si="60">AA364-0.7052</f>
         <v>4.3399999999999994E-2</v>
       </c>
@@ -16100,14 +16110,14 @@
       <c r="M365" s="1">
         <v>30</v>
       </c>
-      <c r="R365" s="1">
+      <c r="R365" s="2">
         <f t="shared" si="57"/>
         <v>0.39000000000000012</v>
       </c>
       <c r="S365" s="1">
         <v>4.03</v>
       </c>
-      <c r="Z365" s="1">
+      <c r="Z365" s="2">
         <f t="shared" ref="Z365" si="61">AA365-0.7052</f>
         <v>-1.319999999999999E-2</v>
       </c>
@@ -16140,14 +16150,14 @@
       <c r="M366" s="1">
         <v>30</v>
       </c>
-      <c r="R366" s="1">
+      <c r="R366" s="2">
         <f t="shared" si="57"/>
         <v>0.22999999999999998</v>
       </c>
       <c r="S366" s="1">
         <v>3.87</v>
       </c>
-      <c r="Z366" s="1">
+      <c r="Z366" s="2">
         <f t="shared" ref="Z366" si="62">AA366-0.7052</f>
         <v>3.1299999999999994E-2</v>
       </c>
@@ -16180,14 +16190,14 @@
       <c r="M367" s="1">
         <v>30</v>
       </c>
-      <c r="R367" s="1">
+      <c r="R367" s="2">
         <f t="shared" si="57"/>
         <v>0.44999999999999973</v>
       </c>
       <c r="S367" s="1">
         <v>4.09</v>
       </c>
-      <c r="Z367" s="1">
+      <c r="Z367" s="2">
         <f t="shared" ref="Z367" si="63">AA367-0.7052</f>
         <v>1.6799999999999926E-2</v>
       </c>
@@ -16220,14 +16230,14 @@
       <c r="M368" s="1">
         <v>30</v>
       </c>
-      <c r="R368" s="1">
+      <c r="R368" s="2">
         <f t="shared" si="57"/>
         <v>0.31999999999999984</v>
       </c>
       <c r="S368" s="1">
         <v>3.96</v>
       </c>
-      <c r="Z368" s="1">
+      <c r="Z368" s="2">
         <f t="shared" ref="Z368" si="64">AA368-0.7052</f>
         <v>3.1999999999999917E-2</v>
       </c>
@@ -16260,14 +16270,14 @@
       <c r="M369" s="1">
         <v>30</v>
       </c>
-      <c r="R369" s="1">
+      <c r="R369" s="2">
         <f t="shared" si="57"/>
         <v>0.35000000000000009</v>
       </c>
       <c r="S369" s="1">
         <v>3.99</v>
       </c>
-      <c r="Z369" s="1">
+      <c r="Z369" s="2">
         <f t="shared" ref="Z369" si="65">AA369-0.7052</f>
         <v>-2.5399999999999978E-2</v>
       </c>
@@ -16300,14 +16310,14 @@
       <c r="M370" s="1">
         <v>30</v>
       </c>
-      <c r="R370" s="1">
+      <c r="R370" s="2">
         <f t="shared" si="57"/>
         <v>0.33999999999999986</v>
       </c>
       <c r="S370" s="1">
         <v>3.98</v>
       </c>
-      <c r="Z370" s="1">
+      <c r="Z370" s="2">
         <f t="shared" ref="Z370" si="66">AA370-0.7052</f>
         <v>-2.6700000000000057E-2</v>
       </c>
@@ -16340,14 +16350,14 @@
       <c r="M371" s="1">
         <v>30</v>
       </c>
-      <c r="R371" s="1">
+      <c r="R371" s="2">
         <f t="shared" si="57"/>
         <v>0.39000000000000012</v>
       </c>
       <c r="S371" s="1">
         <v>4.03</v>
       </c>
-      <c r="Z371" s="1">
+      <c r="Z371" s="2">
         <f t="shared" ref="Z371" si="67">AA371-0.7052</f>
         <v>3.1999999999999806E-3</v>
       </c>
@@ -16380,14 +16390,14 @@
       <c r="M372" s="1">
         <v>30</v>
       </c>
-      <c r="R372" s="1">
+      <c r="R372" s="2">
         <f t="shared" si="57"/>
         <v>0.25999999999999979</v>
       </c>
       <c r="S372" s="1">
         <v>3.9</v>
       </c>
-      <c r="Z372" s="1">
+      <c r="Z372" s="2">
         <f t="shared" ref="Z372" si="68">AA372-0.7052</f>
         <v>1.0499999999999843E-2</v>
       </c>
@@ -16420,14 +16430,14 @@
       <c r="M373" s="1">
         <v>30</v>
       </c>
-      <c r="R373" s="1">
+      <c r="R373" s="2">
         <f t="shared" si="57"/>
         <v>0.37999999999999945</v>
       </c>
       <c r="S373" s="1">
         <v>4.0199999999999996</v>
       </c>
-      <c r="Z373" s="1">
+      <c r="Z373" s="2">
         <f t="shared" ref="Z373" si="69">AA373-0.7052</f>
         <v>8.599999999999941E-3</v>
       </c>
@@ -16460,14 +16470,14 @@
       <c r="M374" s="1">
         <v>30</v>
       </c>
-      <c r="R374" s="1">
+      <c r="R374" s="2">
         <f t="shared" si="57"/>
         <v>0.37999999999999945</v>
       </c>
       <c r="S374" s="1">
         <v>4.0199999999999996</v>
       </c>
-      <c r="Z374" s="1">
+      <c r="Z374" s="2">
         <f t="shared" ref="Z374" si="70">AA374-0.7052</f>
         <v>4.0999999999999925E-3</v>
       </c>
@@ -16500,14 +16510,14 @@
       <c r="M375" s="1">
         <v>30</v>
       </c>
-      <c r="R375" s="1">
+      <c r="R375" s="2">
         <f t="shared" si="57"/>
         <v>0.45999999999999952</v>
       </c>
       <c r="S375" s="1">
         <v>4.0999999999999996</v>
       </c>
-      <c r="Z375" s="1">
+      <c r="Z375" s="2">
         <f t="shared" ref="Z375" si="71">AA375-0.7052</f>
         <v>4.1999999999999815E-3</v>
       </c>
@@ -16540,14 +16550,14 @@
       <c r="M376" s="1">
         <v>30</v>
       </c>
-      <c r="R376" s="1">
+      <c r="R376" s="2">
         <f t="shared" si="57"/>
         <v>0.35000000000000009</v>
       </c>
       <c r="S376" s="1">
         <v>3.99</v>
       </c>
-      <c r="Z376" s="1">
+      <c r="Z376" s="2">
         <f t="shared" ref="Z376" si="72">AA376-0.7052</f>
         <v>-7.4000000000000732E-3</v>
       </c>
@@ -16580,14 +16590,14 @@
       <c r="M377" s="1">
         <v>0</v>
       </c>
-      <c r="R377" s="1">
+      <c r="R377" s="2">
         <f>S377-1.75</f>
         <v>-7.0000000000000062E-2</v>
       </c>
       <c r="S377" s="1">
         <v>1.68</v>
       </c>
-      <c r="Z377" s="1">
+      <c r="Z377" s="2">
         <f>AA377-0.2427</f>
         <v>5.2999999999999992E-3</v>
       </c>
@@ -16620,14 +16630,14 @@
       <c r="M378" s="1">
         <v>0</v>
       </c>
-      <c r="R378" s="1">
+      <c r="R378" s="2">
         <f t="shared" ref="R378:R392" si="73">S378-1.75</f>
         <v>0.25</v>
       </c>
       <c r="S378" s="1">
         <v>2</v>
       </c>
-      <c r="Z378" s="1">
+      <c r="Z378" s="2">
         <f>AA378-0.2427</f>
         <v>6.7600000000000021E-2</v>
       </c>
@@ -16660,14 +16670,14 @@
       <c r="M379" s="1">
         <v>0</v>
       </c>
-      <c r="R379" s="1">
+      <c r="R379" s="2">
         <f t="shared" si="73"/>
         <v>-1.0000000000000009E-2</v>
       </c>
       <c r="S379" s="1">
         <v>1.74</v>
       </c>
-      <c r="Z379" s="1">
+      <c r="Z379" s="2">
         <f t="shared" ref="Z379:Z392" si="74">AA379-0.2427</f>
         <v>3.4400000000000014E-2</v>
       </c>
@@ -16700,14 +16710,14 @@
       <c r="M380" s="1">
         <v>0</v>
       </c>
-      <c r="R380" s="1">
+      <c r="R380" s="2">
         <f t="shared" si="73"/>
         <v>0.1100000000000001</v>
       </c>
       <c r="S380" s="1">
         <v>1.86</v>
       </c>
-      <c r="Z380" s="1">
+      <c r="Z380" s="2">
         <f t="shared" si="74"/>
         <v>7.4499999999999983E-2</v>
       </c>
@@ -16740,14 +16750,14 @@
       <c r="M381" s="1">
         <v>0</v>
       </c>
-      <c r="R381" s="1">
+      <c r="R381" s="2">
         <f t="shared" si="73"/>
         <v>-0.40999999999999992</v>
       </c>
       <c r="S381" s="1">
         <v>1.34</v>
       </c>
-      <c r="Z381" s="1">
+      <c r="Z381" s="2">
         <f t="shared" si="74"/>
         <v>2.1499999999999991E-2</v>
       </c>
@@ -16780,14 +16790,14 @@
       <c r="M382" s="1">
         <v>0</v>
       </c>
-      <c r="R382" s="1">
+      <c r="R382" s="2">
         <f t="shared" si="73"/>
         <v>0.18999999999999995</v>
       </c>
       <c r="S382" s="1">
         <v>1.94</v>
       </c>
-      <c r="Z382" s="1">
+      <c r="Z382" s="2">
         <f t="shared" si="74"/>
         <v>4.8500000000000015E-2</v>
       </c>
@@ -16820,14 +16830,14 @@
       <c r="M383" s="1">
         <v>0</v>
       </c>
-      <c r="R383" s="1">
+      <c r="R383" s="2">
         <f t="shared" si="73"/>
         <v>0.16999999999999993</v>
       </c>
       <c r="S383" s="1">
         <v>1.92</v>
       </c>
-      <c r="Z383" s="1">
+      <c r="Z383" s="2">
         <f t="shared" si="74"/>
         <v>9.0599999999999986E-2</v>
       </c>
@@ -16860,14 +16870,14 @@
       <c r="M384" s="1">
         <v>0</v>
       </c>
-      <c r="R384" s="1">
+      <c r="R384" s="2">
         <f t="shared" si="73"/>
         <v>0.18999999999999995</v>
       </c>
       <c r="S384" s="1">
         <v>1.94</v>
       </c>
-      <c r="Z384" s="1">
+      <c r="Z384" s="2">
         <f t="shared" si="74"/>
         <v>8.1800000000000012E-2</v>
       </c>
@@ -16900,14 +16910,14 @@
       <c r="M385" s="1">
         <v>0</v>
       </c>
-      <c r="R385" s="1">
+      <c r="R385" s="2">
         <f t="shared" si="73"/>
         <v>2.0000000000000018E-2</v>
       </c>
       <c r="S385" s="1">
         <v>1.77</v>
       </c>
-      <c r="Z385" s="1">
+      <c r="Z385" s="2">
         <f t="shared" si="74"/>
         <v>5.4900000000000032E-2</v>
       </c>
@@ -16940,14 +16950,14 @@
       <c r="M386" s="1">
         <v>0</v>
       </c>
-      <c r="R386" s="1">
+      <c r="R386" s="2">
         <f t="shared" si="73"/>
         <v>3.0000000000000027E-2</v>
       </c>
       <c r="S386" s="1">
         <v>1.78</v>
       </c>
-      <c r="Z386" s="1">
+      <c r="Z386" s="2">
         <f t="shared" si="74"/>
         <v>5.460000000000001E-2</v>
       </c>
@@ -16980,14 +16990,14 @@
       <c r="M387" s="1">
         <v>0</v>
       </c>
-      <c r="R387" s="1">
+      <c r="R387" s="2">
         <f t="shared" si="73"/>
         <v>6.0000000000000053E-2</v>
       </c>
       <c r="S387" s="1">
         <v>1.81</v>
       </c>
-      <c r="Z387" s="1">
+      <c r="Z387" s="2">
         <f t="shared" si="74"/>
         <v>6.5700000000000008E-2</v>
       </c>
@@ -17020,14 +17030,14 @@
       <c r="M388" s="1">
         <v>0</v>
       </c>
-      <c r="R388" s="1">
+      <c r="R388" s="2">
         <f t="shared" si="73"/>
         <v>-0.18999999999999995</v>
       </c>
       <c r="S388" s="1">
         <v>1.56</v>
       </c>
-      <c r="Z388" s="1">
+      <c r="Z388" s="2">
         <f t="shared" si="74"/>
         <v>4.9799999999999983E-2</v>
       </c>
@@ -17060,14 +17070,14 @@
       <c r="M389" s="1">
         <v>0</v>
       </c>
-      <c r="R389" s="1">
+      <c r="R389" s="2">
         <f t="shared" si="73"/>
         <v>0.16999999999999993</v>
       </c>
       <c r="S389" s="1">
         <v>1.92</v>
       </c>
-      <c r="Z389" s="1">
+      <c r="Z389" s="2">
         <f t="shared" si="74"/>
         <v>8.5800000000000015E-2</v>
       </c>
@@ -17100,14 +17110,14 @@
       <c r="M390" s="1">
         <v>0</v>
       </c>
-      <c r="R390" s="1">
+      <c r="R390" s="2">
         <f t="shared" si="73"/>
         <v>0.1100000000000001</v>
       </c>
       <c r="S390" s="1">
         <v>1.86</v>
       </c>
-      <c r="Z390" s="1">
+      <c r="Z390" s="2">
         <f t="shared" si="74"/>
         <v>6.9700000000000012E-2</v>
       </c>
@@ -17140,14 +17150,14 @@
       <c r="M391" s="1">
         <v>0</v>
       </c>
-      <c r="R391" s="1">
+      <c r="R391" s="2">
         <f t="shared" si="73"/>
         <v>-5.0000000000000044E-2</v>
       </c>
       <c r="S391" s="1">
         <v>1.7</v>
       </c>
-      <c r="Z391" s="1">
+      <c r="Z391" s="2">
         <f t="shared" si="74"/>
         <v>3.2400000000000012E-2</v>
       </c>
@@ -17180,14 +17190,14 @@
       <c r="M392" s="1">
         <v>0</v>
       </c>
-      <c r="R392" s="1">
+      <c r="R392" s="2">
         <f t="shared" si="73"/>
         <v>-0.31000000000000005</v>
       </c>
       <c r="S392" s="1">
         <v>1.44</v>
       </c>
-      <c r="Z392" s="1">
+      <c r="Z392" s="2">
         <f t="shared" si="74"/>
         <v>8.299999999999999E-2</v>
       </c>
@@ -17220,14 +17230,14 @@
       <c r="M393" s="1">
         <v>5</v>
       </c>
-      <c r="R393" s="1">
+      <c r="R393" s="2">
         <f>S393-1.75</f>
         <v>0.37999999999999989</v>
       </c>
       <c r="S393" s="1">
         <v>2.13</v>
       </c>
-      <c r="Z393" s="1">
+      <c r="Z393" s="2">
         <f>AA393-0.3332</f>
         <v>6.5999999999999948E-3</v>
       </c>
@@ -17260,14 +17270,14 @@
       <c r="M394" s="1">
         <v>5</v>
       </c>
-      <c r="R394" s="1">
+      <c r="R394" s="2">
         <f t="shared" ref="R394:R408" si="75">S394-1.75</f>
         <v>0.60999999999999988</v>
       </c>
       <c r="S394" s="1">
         <v>2.36</v>
       </c>
-      <c r="Z394" s="1">
+      <c r="Z394" s="2">
         <f>AA394-0.3332</f>
         <v>8.6799999999999988E-2</v>
       </c>
@@ -17300,14 +17310,14 @@
       <c r="M395" s="1">
         <v>5</v>
       </c>
-      <c r="R395" s="1">
+      <c r="R395" s="2">
         <f t="shared" si="75"/>
         <v>0.37999999999999989</v>
       </c>
       <c r="S395" s="1">
         <v>2.13</v>
       </c>
-      <c r="Z395" s="1">
+      <c r="Z395" s="2">
         <f t="shared" ref="Z395:Z408" si="76">AA395-0.3332</f>
         <v>4.6700000000000019E-2</v>
       </c>
@@ -17340,14 +17350,14 @@
       <c r="M396" s="1">
         <v>5</v>
       </c>
-      <c r="R396" s="1">
+      <c r="R396" s="2">
         <f t="shared" si="75"/>
         <v>0.49000000000000021</v>
       </c>
       <c r="S396" s="1">
         <v>2.2400000000000002</v>
       </c>
-      <c r="Z396" s="1">
+      <c r="Z396" s="2">
         <f t="shared" si="76"/>
         <v>7.350000000000001E-2</v>
       </c>
@@ -17380,14 +17390,14 @@
       <c r="M397" s="1">
         <v>5</v>
       </c>
-      <c r="R397" s="1">
+      <c r="R397" s="2">
         <f t="shared" si="75"/>
         <v>0.12999999999999989</v>
       </c>
       <c r="S397" s="1">
         <v>1.88</v>
       </c>
-      <c r="Z397" s="1">
+      <c r="Z397" s="2">
         <f t="shared" si="76"/>
         <v>2.899999999999997E-2</v>
       </c>
@@ -17420,14 +17430,14 @@
       <c r="M398" s="1">
         <v>5</v>
       </c>
-      <c r="R398" s="1">
+      <c r="R398" s="2">
         <f t="shared" si="75"/>
         <v>0.5299999999999998</v>
       </c>
       <c r="S398" s="1">
         <v>2.2799999999999998</v>
       </c>
-      <c r="Z398" s="1">
+      <c r="Z398" s="2">
         <f t="shared" si="76"/>
         <v>5.5499999999999994E-2</v>
       </c>
@@ -17460,14 +17470,14 @@
       <c r="M399" s="1">
         <v>5</v>
       </c>
-      <c r="R399" s="1">
+      <c r="R399" s="2">
         <f t="shared" si="75"/>
         <v>0.54</v>
       </c>
       <c r="S399" s="1">
         <v>2.29</v>
       </c>
-      <c r="Z399" s="1">
+      <c r="Z399" s="2">
         <f t="shared" si="76"/>
         <v>9.4099999999999961E-2</v>
       </c>
@@ -17500,14 +17510,14 @@
       <c r="M400" s="1">
         <v>5</v>
       </c>
-      <c r="R400" s="1">
+      <c r="R400" s="2">
         <f t="shared" si="75"/>
         <v>0.56000000000000005</v>
       </c>
       <c r="S400" s="1">
         <v>2.31</v>
       </c>
-      <c r="Z400" s="1">
+      <c r="Z400" s="2">
         <f t="shared" si="76"/>
         <v>8.4600000000000009E-2</v>
       </c>
@@ -17540,14 +17550,14 @@
       <c r="M401" s="1">
         <v>5</v>
       </c>
-      <c r="R401" s="1">
+      <c r="R401" s="2">
         <f t="shared" si="75"/>
         <v>0.43999999999999995</v>
       </c>
       <c r="S401" s="1">
         <v>2.19</v>
       </c>
-      <c r="Z401" s="1">
+      <c r="Z401" s="2">
         <f t="shared" si="76"/>
         <v>4.4300000000000006E-2</v>
       </c>
@@ -17580,14 +17590,14 @@
       <c r="M402" s="1">
         <v>5</v>
       </c>
-      <c r="R402" s="1">
+      <c r="R402" s="2">
         <f t="shared" si="75"/>
         <v>0.43999999999999995</v>
       </c>
       <c r="S402" s="1">
         <v>2.19</v>
       </c>
-      <c r="Z402" s="1">
+      <c r="Z402" s="2">
         <f t="shared" si="76"/>
         <v>4.2100000000000026E-2</v>
       </c>
@@ -17620,14 +17630,14 @@
       <c r="M403" s="1">
         <v>5</v>
       </c>
-      <c r="R403" s="1">
+      <c r="R403" s="2">
         <f t="shared" si="75"/>
         <v>0.48</v>
       </c>
       <c r="S403" s="1">
         <v>2.23</v>
       </c>
-      <c r="Z403" s="1">
+      <c r="Z403" s="2">
         <f t="shared" si="76"/>
         <v>6.3699999999999979E-2</v>
       </c>
@@ -17660,14 +17670,14 @@
       <c r="M404" s="1">
         <v>5</v>
       </c>
-      <c r="R404" s="1">
+      <c r="R404" s="2">
         <f t="shared" si="75"/>
         <v>0.31999999999999984</v>
       </c>
       <c r="S404" s="1">
         <v>2.0699999999999998</v>
       </c>
-      <c r="Z404" s="1">
+      <c r="Z404" s="2">
         <f t="shared" si="76"/>
         <v>5.4200000000000026E-2</v>
       </c>
@@ -17700,14 +17710,14 @@
       <c r="M405" s="1">
         <v>5</v>
       </c>
-      <c r="R405" s="1">
+      <c r="R405" s="2">
         <f t="shared" si="75"/>
         <v>0.54</v>
       </c>
       <c r="S405" s="1">
         <v>2.29</v>
       </c>
-      <c r="Z405" s="1">
+      <c r="Z405" s="2">
         <f t="shared" si="76"/>
         <v>9.0899999999999981E-2</v>
       </c>
@@ -17740,14 +17750,14 @@
       <c r="M406" s="1">
         <v>5</v>
       </c>
-      <c r="R406" s="1">
+      <c r="R406" s="2">
         <f t="shared" si="75"/>
         <v>0.4700000000000002</v>
       </c>
       <c r="S406" s="1">
         <v>2.2200000000000002</v>
       </c>
-      <c r="Z406" s="1">
+      <c r="Z406" s="2">
         <f t="shared" si="76"/>
         <v>6.3500000000000001E-2</v>
       </c>
@@ -17780,14 +17790,14 @@
       <c r="M407" s="1">
         <v>5</v>
       </c>
-      <c r="R407" s="1">
+      <c r="R407" s="2">
         <f t="shared" si="75"/>
         <v>0.41000000000000014</v>
       </c>
       <c r="S407" s="1">
         <v>2.16</v>
       </c>
-      <c r="Z407" s="1">
+      <c r="Z407" s="2">
         <f t="shared" si="76"/>
         <v>2.250000000000002E-2</v>
       </c>
@@ -17820,14 +17830,14 @@
       <c r="M408" s="1">
         <v>5</v>
       </c>
-      <c r="R408" s="1">
+      <c r="R408" s="2">
         <f t="shared" si="75"/>
         <v>0.18999999999999995</v>
       </c>
       <c r="S408" s="1">
         <v>1.94</v>
       </c>
-      <c r="Z408" s="1">
+      <c r="Z408" s="2">
         <f t="shared" si="76"/>
         <v>7.8199999999999992E-2</v>
       </c>
@@ -17860,14 +17870,14 @@
       <c r="M409" s="1">
         <v>10</v>
       </c>
-      <c r="R409" s="1">
+      <c r="R409" s="2">
         <f>S409-2.43</f>
         <v>0.12999999999999989</v>
       </c>
       <c r="S409" s="1">
         <v>2.56</v>
       </c>
-      <c r="Z409" s="1">
+      <c r="Z409" s="2">
         <f>AA409-0.4529</f>
         <v>-1.3000000000000012E-2</v>
       </c>
@@ -17900,14 +17910,14 @@
       <c r="M410" s="1">
         <v>10</v>
       </c>
-      <c r="R410" s="1">
+      <c r="R410" s="2">
         <f t="shared" ref="R410:R424" si="77">S410-2.43</f>
         <v>0.25999999999999979</v>
       </c>
       <c r="S410" s="1">
         <v>2.69</v>
       </c>
-      <c r="Z410" s="1">
+      <c r="Z410" s="2">
         <f>AA410-0.4529</f>
         <v>7.6600000000000057E-2</v>
       </c>
@@ -17940,14 +17950,14 @@
       <c r="M411" s="1">
         <v>10</v>
       </c>
-      <c r="R411" s="1">
+      <c r="R411" s="2">
         <f t="shared" si="77"/>
         <v>9.9999999999999645E-2</v>
       </c>
       <c r="S411" s="1">
         <v>2.5299999999999998</v>
       </c>
-      <c r="Z411" s="1">
+      <c r="Z411" s="2">
         <f t="shared" ref="Z411:Z424" si="78">AA411-0.4529</f>
         <v>5.1099999999999979E-2</v>
       </c>
@@ -17980,14 +17990,14 @@
       <c r="M412" s="1">
         <v>10</v>
       </c>
-      <c r="R412" s="1">
+      <c r="R412" s="2">
         <f t="shared" si="77"/>
         <v>0.17999999999999972</v>
       </c>
       <c r="S412" s="1">
         <v>2.61</v>
       </c>
-      <c r="Z412" s="1">
+      <c r="Z412" s="2">
         <f t="shared" si="78"/>
         <v>5.6199999999999972E-2</v>
       </c>
@@ -18020,14 +18030,14 @@
       <c r="M413" s="1">
         <v>10</v>
       </c>
-      <c r="R413" s="1">
+      <c r="R413" s="2">
         <f t="shared" si="77"/>
         <v>-5.0000000000000266E-2</v>
       </c>
       <c r="S413" s="1">
         <v>2.38</v>
       </c>
-      <c r="Z413" s="1">
+      <c r="Z413" s="2">
         <f t="shared" si="78"/>
         <v>2.300000000000002E-2</v>
       </c>
@@ -18060,14 +18070,14 @@
       <c r="M414" s="1">
         <v>10</v>
       </c>
-      <c r="R414" s="1">
+      <c r="R414" s="2">
         <f t="shared" si="77"/>
         <v>0.20999999999999996</v>
       </c>
       <c r="S414" s="1">
         <v>2.64</v>
       </c>
-      <c r="Z414" s="1">
+      <c r="Z414" s="2">
         <f t="shared" si="78"/>
         <v>5.0500000000000045E-2</v>
       </c>
@@ -18100,14 +18110,14 @@
       <c r="M415" s="1">
         <v>10</v>
       </c>
-      <c r="R415" s="1">
+      <c r="R415" s="2">
         <f t="shared" si="77"/>
         <v>0.25</v>
       </c>
       <c r="S415" s="1">
         <v>2.68</v>
       </c>
-      <c r="Z415" s="1">
+      <c r="Z415" s="2">
         <f t="shared" si="78"/>
         <v>7.1899999999999908E-2</v>
       </c>
@@ -18140,14 +18150,14 @@
       <c r="M416" s="1">
         <v>10</v>
       </c>
-      <c r="R416" s="1">
+      <c r="R416" s="2">
         <f t="shared" si="77"/>
         <v>0.23999999999999977</v>
       </c>
       <c r="S416" s="1">
         <v>2.67</v>
       </c>
-      <c r="Z416" s="1">
+      <c r="Z416" s="2">
         <f t="shared" si="78"/>
         <v>6.5900000000000014E-2</v>
       </c>
@@ -18180,14 +18190,14 @@
       <c r="M417" s="1">
         <v>10</v>
       </c>
-      <c r="R417" s="1">
+      <c r="R417" s="2">
         <f t="shared" si="77"/>
         <v>0.1599999999999997</v>
       </c>
       <c r="S417" s="1">
         <v>2.59</v>
       </c>
-      <c r="Z417" s="1">
+      <c r="Z417" s="2">
         <f t="shared" si="78"/>
         <v>3.7700000000000011E-2</v>
       </c>
@@ -18220,14 +18230,14 @@
       <c r="M418" s="1">
         <v>10</v>
       </c>
-      <c r="R418" s="1">
+      <c r="R418" s="2">
         <f t="shared" si="77"/>
         <v>0.16999999999999993</v>
       </c>
       <c r="S418" s="1">
         <v>2.6</v>
       </c>
-      <c r="Z418" s="1">
+      <c r="Z418" s="2">
         <f t="shared" si="78"/>
         <v>2.8699999999999948E-2</v>
       </c>
@@ -18260,14 +18270,14 @@
       <c r="M419" s="1">
         <v>10</v>
       </c>
-      <c r="R419" s="1">
+      <c r="R419" s="2">
         <f t="shared" si="77"/>
         <v>0.18999999999999995</v>
       </c>
       <c r="S419" s="1">
         <v>2.62</v>
       </c>
-      <c r="Z419" s="1">
+      <c r="Z419" s="2">
         <f t="shared" si="78"/>
         <v>6.090000000000001E-2</v>
       </c>
@@ -18300,14 +18310,14 @@
       <c r="M420" s="1">
         <v>10</v>
       </c>
-      <c r="R420" s="1">
+      <c r="R420" s="2">
         <f t="shared" si="77"/>
         <v>9.9999999999999645E-2</v>
       </c>
       <c r="S420" s="1">
         <v>2.5299999999999998</v>
       </c>
-      <c r="Z420" s="1">
+      <c r="Z420" s="2">
         <f t="shared" si="78"/>
         <v>3.8999999999999979E-2</v>
       </c>
@@ -18340,14 +18350,14 @@
       <c r="M421" s="1">
         <v>10</v>
       </c>
-      <c r="R421" s="1">
+      <c r="R421" s="2">
         <f t="shared" si="77"/>
         <v>0.23999999999999977</v>
       </c>
       <c r="S421" s="1">
         <v>2.67</v>
       </c>
-      <c r="Z421" s="1">
+      <c r="Z421" s="2">
         <f t="shared" si="78"/>
         <v>7.0299999999999974E-2</v>
       </c>
@@ -18380,14 +18390,14 @@
       <c r="M422" s="1">
         <v>10</v>
       </c>
-      <c r="R422" s="1">
+      <c r="R422" s="2">
         <f t="shared" si="77"/>
         <v>0.17999999999999972</v>
       </c>
       <c r="S422" s="1">
         <v>2.61</v>
       </c>
-      <c r="Z422" s="1">
+      <c r="Z422" s="2">
         <f t="shared" si="78"/>
         <v>5.319999999999997E-2</v>
       </c>
@@ -18420,14 +18430,14 @@
       <c r="M423" s="1">
         <v>10</v>
       </c>
-      <c r="R423" s="1">
+      <c r="R423" s="2">
         <f t="shared" si="77"/>
         <v>0.14999999999999991</v>
       </c>
       <c r="S423" s="1">
         <v>2.58</v>
       </c>
-      <c r="Z423" s="1">
+      <c r="Z423" s="2">
         <f t="shared" si="78"/>
         <v>1.5099999999999947E-2</v>
       </c>
@@ -18460,14 +18470,14 @@
       <c r="M424" s="1">
         <v>10</v>
       </c>
-      <c r="R424" s="1">
+      <c r="R424" s="2">
         <f t="shared" si="77"/>
         <v>-1.0000000000000231E-2</v>
       </c>
       <c r="S424" s="1">
         <v>2.42</v>
       </c>
-      <c r="Z424" s="1">
+      <c r="Z424" s="2">
         <f t="shared" si="78"/>
         <v>6.6199999999999981E-2</v>
       </c>
@@ -18500,14 +18510,14 @@
       <c r="M425" s="1">
         <v>15</v>
       </c>
-      <c r="R425" s="1">
+      <c r="R425" s="2">
         <f>S425-2.77</f>
         <v>0.20000000000000018</v>
       </c>
       <c r="S425" s="1">
         <v>2.97</v>
       </c>
-      <c r="Z425" s="1">
+      <c r="Z425" s="2">
         <f>AA425-0.5649</f>
         <v>-3.0299999999999994E-2</v>
       </c>
@@ -18540,14 +18550,14 @@
       <c r="M426" s="1">
         <v>15</v>
       </c>
-      <c r="R426" s="1">
+      <c r="R426" s="2">
         <f t="shared" ref="R426:R440" si="79">S426-2.77</f>
         <v>0.20999999999999996</v>
       </c>
       <c r="S426" s="1">
         <v>2.98</v>
       </c>
-      <c r="Z426" s="1">
+      <c r="Z426" s="2">
         <f>AA426-0.5649</f>
         <v>3.9000000000000035E-2</v>
       </c>
@@ -18580,14 +18590,14 @@
       <c r="M427" s="1">
         <v>15</v>
       </c>
-      <c r="R427" s="1">
+      <c r="R427" s="2">
         <f t="shared" si="79"/>
         <v>0.14000000000000012</v>
       </c>
       <c r="S427" s="1">
         <v>2.91</v>
       </c>
-      <c r="Z427" s="1">
+      <c r="Z427" s="2">
         <f t="shared" ref="Z427:Z440" si="80">AA427-0.5649</f>
         <v>5.4000000000000048E-2</v>
       </c>
@@ -18620,14 +18630,14 @@
       <c r="M428" s="1">
         <v>15</v>
       </c>
-      <c r="R428" s="1">
+      <c r="R428" s="2">
         <f t="shared" si="79"/>
         <v>0.20000000000000018</v>
       </c>
       <c r="S428" s="1">
         <v>2.97</v>
       </c>
-      <c r="Z428" s="1">
+      <c r="Z428" s="2">
         <f t="shared" si="80"/>
         <v>4.6900000000000053E-2</v>
       </c>
@@ -18660,14 +18670,14 @@
       <c r="M429" s="1">
         <v>15</v>
       </c>
-      <c r="R429" s="1">
+      <c r="R429" s="2">
         <f t="shared" si="79"/>
         <v>6.999999999999984E-2</v>
       </c>
       <c r="S429" s="1">
         <v>2.84</v>
       </c>
-      <c r="Z429" s="1">
+      <c r="Z429" s="2">
         <f t="shared" si="80"/>
         <v>6.8000000000000282E-3</v>
       </c>
@@ -18700,14 +18710,14 @@
       <c r="M430" s="1">
         <v>15</v>
       </c>
-      <c r="R430" s="1">
+      <c r="R430" s="2">
         <f t="shared" si="79"/>
         <v>0.20000000000000018</v>
       </c>
       <c r="S430" s="1">
         <v>2.97</v>
       </c>
-      <c r="Z430" s="1">
+      <c r="Z430" s="2">
         <f t="shared" si="80"/>
         <v>4.8500000000000099E-2</v>
       </c>
@@ -18740,14 +18750,14 @@
       <c r="M431" s="1">
         <v>15</v>
       </c>
-      <c r="R431" s="1">
+      <c r="R431" s="2">
         <f t="shared" si="79"/>
         <v>0.27</v>
       </c>
       <c r="S431" s="1">
         <v>3.04</v>
       </c>
-      <c r="Z431" s="1">
+      <c r="Z431" s="2">
         <f t="shared" si="80"/>
         <v>4.0000000000000036E-2</v>
       </c>
@@ -18780,14 +18790,14 @@
       <c r="M432" s="1">
         <v>15</v>
       </c>
-      <c r="R432" s="1">
+      <c r="R432" s="2">
         <f t="shared" si="79"/>
         <v>0.25</v>
       </c>
       <c r="S432" s="1">
         <v>3.02</v>
       </c>
-      <c r="Z432" s="1">
+      <c r="Z432" s="2">
         <f t="shared" si="80"/>
         <v>5.3200000000000025E-2</v>
       </c>
@@ -18820,14 +18830,14 @@
       <c r="M433" s="1">
         <v>15</v>
       </c>
-      <c r="R433" s="1">
+      <c r="R433" s="2">
         <f t="shared" si="79"/>
         <v>0.2200000000000002</v>
       </c>
       <c r="S433" s="1">
         <v>2.99</v>
       </c>
-      <c r="Z433" s="1">
+      <c r="Z433" s="2">
         <f t="shared" si="80"/>
         <v>3.0999999999999917E-3</v>
       </c>
@@ -18860,14 +18870,14 @@
       <c r="M434" s="1">
         <v>15</v>
       </c>
-      <c r="R434" s="1">
+      <c r="R434" s="2">
         <f t="shared" si="79"/>
         <v>0.2200000000000002</v>
       </c>
       <c r="S434" s="1">
         <v>2.99</v>
       </c>
-      <c r="Z434" s="1">
+      <c r="Z434" s="2">
         <f t="shared" si="80"/>
         <v>2.7000000000000357E-3</v>
       </c>
@@ -18900,14 +18910,14 @@
       <c r="M435" s="1">
         <v>15</v>
       </c>
-      <c r="R435" s="1">
+      <c r="R435" s="2">
         <f t="shared" si="79"/>
         <v>0.23999999999999977</v>
       </c>
       <c r="S435" s="1">
         <v>3.01</v>
       </c>
-      <c r="Z435" s="1">
+      <c r="Z435" s="2">
         <f t="shared" si="80"/>
         <v>3.0500000000000083E-2</v>
       </c>
@@ -18940,14 +18950,14 @@
       <c r="M436" s="1">
         <v>15</v>
       </c>
-      <c r="R436" s="1">
+      <c r="R436" s="2">
         <f t="shared" si="79"/>
         <v>0.16000000000000014</v>
       </c>
       <c r="S436" s="1">
         <v>2.93</v>
       </c>
-      <c r="Z436" s="1">
+      <c r="Z436" s="2">
         <f t="shared" si="80"/>
         <v>3.4700000000000064E-2</v>
       </c>
@@ -18980,14 +18990,14 @@
       <c r="M437" s="1">
         <v>15</v>
       </c>
-      <c r="R437" s="1">
+      <c r="R437" s="2">
         <f t="shared" si="79"/>
         <v>0.25999999999999979</v>
       </c>
       <c r="S437" s="1">
         <v>3.03</v>
       </c>
-      <c r="Z437" s="1">
+      <c r="Z437" s="2">
         <f t="shared" si="80"/>
         <v>3.4600000000000075E-2</v>
       </c>
@@ -19020,14 +19030,14 @@
       <c r="M438" s="1">
         <v>15</v>
       </c>
-      <c r="R438" s="1">
+      <c r="R438" s="2">
         <f t="shared" si="79"/>
         <v>0.20999999999999996</v>
       </c>
       <c r="S438" s="1">
         <v>2.98</v>
       </c>
-      <c r="Z438" s="1">
+      <c r="Z438" s="2">
         <f t="shared" si="80"/>
         <v>2.0700000000000052E-2</v>
       </c>
@@ -19060,14 +19070,14 @@
       <c r="M439" s="1">
         <v>15</v>
       </c>
-      <c r="R439" s="1">
+      <c r="R439" s="2">
         <f t="shared" si="79"/>
         <v>0.20999999999999996</v>
       </c>
       <c r="S439" s="1">
         <v>2.98</v>
       </c>
-      <c r="Z439" s="1">
+      <c r="Z439" s="2">
         <f t="shared" si="80"/>
         <v>-4.1999999999999815E-3</v>
       </c>
@@ -19100,14 +19110,14 @@
       <c r="M440" s="1">
         <v>15</v>
       </c>
-      <c r="R440" s="1">
+      <c r="R440" s="2">
         <f t="shared" si="79"/>
         <v>0.10999999999999988</v>
       </c>
       <c r="S440" s="1">
         <v>2.88</v>
       </c>
-      <c r="Z440" s="1">
+      <c r="Z440" s="2">
         <f t="shared" si="80"/>
         <v>3.9100000000000024E-2</v>
       </c>
@@ -19140,14 +19150,14 @@
       <c r="M441" s="1">
         <v>20</v>
       </c>
-      <c r="R441" s="1">
+      <c r="R441" s="2">
         <f>S441-3.1</f>
         <v>0.25999999999999979</v>
       </c>
       <c r="S441" s="1">
         <v>3.36</v>
       </c>
-      <c r="Z441" s="1">
+      <c r="Z441" s="2">
         <f>AA441-0.6516</f>
         <v>-4.1100000000000025E-2</v>
       </c>
@@ -19180,14 +19190,14 @@
       <c r="M442" s="1">
         <v>20</v>
       </c>
-      <c r="R442" s="1">
+      <c r="R442" s="2">
         <f t="shared" ref="R442:R456" si="81">S442-3.1</f>
         <v>0.10999999999999988</v>
       </c>
       <c r="S442" s="1">
         <v>3.21</v>
       </c>
-      <c r="Z442" s="1">
+      <c r="Z442" s="2">
         <f>AA442-0.6516</f>
         <v>-5.6000000000000494E-3</v>
       </c>
@@ -19220,14 +19230,14 @@
       <c r="M443" s="1">
         <v>20</v>
       </c>
-      <c r="R443" s="1">
+      <c r="R443" s="2">
         <f t="shared" si="81"/>
         <v>0.16999999999999993</v>
       </c>
       <c r="S443" s="1">
         <v>3.27</v>
       </c>
-      <c r="Z443" s="1">
+      <c r="Z443" s="2">
         <f t="shared" ref="Z443:Z456" si="82">AA443-0.6516</f>
         <v>3.4200000000000008E-2</v>
       </c>
@@ -19260,14 +19270,14 @@
       <c r="M444" s="1">
         <v>20</v>
       </c>
-      <c r="R444" s="1">
+      <c r="R444" s="2">
         <f t="shared" si="81"/>
         <v>0.20999999999999996</v>
       </c>
       <c r="S444" s="1">
         <v>3.31</v>
       </c>
-      <c r="Z444" s="1">
+      <c r="Z444" s="2">
         <f t="shared" si="82"/>
         <v>1.2700000000000156E-2</v>
       </c>
@@ -19300,14 +19310,14 @@
       <c r="M445" s="1">
         <v>20</v>
       </c>
-      <c r="R445" s="1">
+      <c r="R445" s="2">
         <f t="shared" si="81"/>
         <v>0.16999999999999993</v>
       </c>
       <c r="S445" s="1">
         <v>3.27</v>
       </c>
-      <c r="Z445" s="1">
+      <c r="Z445" s="2">
         <f t="shared" si="82"/>
         <v>-3.0999999999999917E-3</v>
       </c>
@@ -19340,14 +19350,14 @@
       <c r="M446" s="1">
         <v>20</v>
       </c>
-      <c r="R446" s="1">
+      <c r="R446" s="2">
         <f t="shared" si="81"/>
         <v>0.17999999999999972</v>
       </c>
       <c r="S446" s="1">
         <v>3.28</v>
       </c>
-      <c r="Z446" s="1">
+      <c r="Z446" s="2">
         <f t="shared" si="82"/>
         <v>2.3599999999999954E-2</v>
       </c>
@@ -19380,14 +19390,14 @@
       <c r="M447" s="1">
         <v>20</v>
       </c>
-      <c r="R447" s="1">
+      <c r="R447" s="2">
         <f t="shared" si="81"/>
         <v>0.2799999999999998</v>
       </c>
       <c r="S447" s="1">
         <v>3.38</v>
       </c>
-      <c r="Z447" s="1">
+      <c r="Z447" s="2">
         <f t="shared" si="82"/>
         <v>2.9000000000001247E-3</v>
       </c>
@@ -19420,14 +19430,14 @@
       <c r="M448" s="1">
         <v>20</v>
       </c>
-      <c r="R448" s="1">
+      <c r="R448" s="2">
         <f t="shared" si="81"/>
         <v>0.22999999999999998</v>
       </c>
       <c r="S448" s="1">
         <v>3.33</v>
       </c>
-      <c r="Z448" s="1">
+      <c r="Z448" s="2">
         <f t="shared" si="82"/>
         <v>2.2199999999999998E-2</v>
       </c>
@@ -19460,14 +19470,14 @@
       <c r="M449" s="1">
         <v>20</v>
       </c>
-      <c r="R449" s="1">
+      <c r="R449" s="2">
         <f t="shared" si="81"/>
         <v>0.23999999999999977</v>
       </c>
       <c r="S449" s="1">
         <v>3.34</v>
       </c>
-      <c r="Z449" s="1">
+      <c r="Z449" s="2">
         <f t="shared" si="82"/>
         <v>-2.5599999999999956E-2</v>
       </c>
@@ -19500,14 +19510,14 @@
       <c r="M450" s="1">
         <v>20</v>
       </c>
-      <c r="R450" s="1">
+      <c r="R450" s="2">
         <f t="shared" si="81"/>
         <v>0.23999999999999977</v>
       </c>
       <c r="S450" s="1">
         <v>3.34</v>
       </c>
-      <c r="Z450" s="1">
+      <c r="Z450" s="2">
         <f t="shared" si="82"/>
         <v>-2.9299999999999993E-2</v>
       </c>
@@ -19540,14 +19550,14 @@
       <c r="M451" s="1">
         <v>20</v>
       </c>
-      <c r="R451" s="1">
+      <c r="R451" s="2">
         <f t="shared" si="81"/>
         <v>0.25</v>
       </c>
       <c r="S451" s="1">
         <v>3.35</v>
       </c>
-      <c r="Z451" s="1">
+      <c r="Z451" s="2">
         <f t="shared" si="82"/>
         <v>-2.4999999999999467E-3</v>
       </c>
@@ -19580,14 +19590,14 @@
       <c r="M452" s="1">
         <v>20</v>
       </c>
-      <c r="R452" s="1">
+      <c r="R452" s="2">
         <f t="shared" si="81"/>
         <v>0.17999999999999972</v>
       </c>
       <c r="S452" s="1">
         <v>3.28</v>
       </c>
-      <c r="Z452" s="1">
+      <c r="Z452" s="2">
         <f t="shared" si="82"/>
         <v>1.5800000000000036E-2</v>
       </c>
@@ -19620,14 +19630,14 @@
       <c r="M453" s="1">
         <v>20</v>
       </c>
-      <c r="R453" s="1">
+      <c r="R453" s="2">
         <f t="shared" si="81"/>
         <v>0.25999999999999979</v>
       </c>
       <c r="S453" s="1">
         <v>3.36</v>
       </c>
-      <c r="Z453" s="1">
+      <c r="Z453" s="2">
         <f t="shared" si="82"/>
         <v>1.9000000000000128E-3</v>
       </c>
@@ -19660,14 +19670,14 @@
       <c r="M454" s="1">
         <v>20</v>
       </c>
-      <c r="R454" s="1">
+      <c r="R454" s="2">
         <f t="shared" si="81"/>
         <v>0.21999999999999975</v>
       </c>
       <c r="S454" s="1">
         <v>3.32</v>
       </c>
-      <c r="Z454" s="1">
+      <c r="Z454" s="2">
         <f t="shared" si="82"/>
         <v>-1.6299999999999981E-2</v>
       </c>
@@ -19700,14 +19710,14 @@
       <c r="M455" s="1">
         <v>20</v>
       </c>
-      <c r="R455" s="1">
+      <c r="R455" s="2">
         <f t="shared" si="81"/>
         <v>0.25</v>
       </c>
       <c r="S455" s="1">
         <v>3.35</v>
       </c>
-      <c r="Z455" s="1">
+      <c r="Z455" s="2">
         <f t="shared" si="82"/>
         <v>-2.5899999999999923E-2</v>
       </c>
@@ -19740,14 +19750,14 @@
       <c r="M456" s="1">
         <v>20</v>
       </c>
-      <c r="R456" s="1">
+      <c r="R456" s="2">
         <f t="shared" si="81"/>
         <v>0.17999999999999972</v>
       </c>
       <c r="S456" s="1">
         <v>3.28</v>
       </c>
-      <c r="Z456" s="1">
+      <c r="Z456" s="2">
         <f t="shared" si="82"/>
         <v>9.8000000000000309E-3</v>
       </c>
@@ -19780,14 +19790,14 @@
       <c r="M457" s="1">
         <v>25</v>
       </c>
-      <c r="R457" s="1">
+      <c r="R457" s="2">
         <f>S457-3.43</f>
         <v>0.25999999999999979</v>
       </c>
       <c r="S457" s="1">
         <v>3.69</v>
       </c>
-      <c r="Z457" s="1">
+      <c r="Z457" s="2">
         <f>AA457-0.7116</f>
         <v>-4.5399999999999996E-2</v>
       </c>
@@ -19820,14 +19830,14 @@
       <c r="M458" s="1">
         <v>25</v>
       </c>
-      <c r="R458" s="1">
+      <c r="R458" s="2">
         <f t="shared" ref="R458:R472" si="83">S458-3.43</f>
         <v>-6.0000000000000053E-2</v>
       </c>
       <c r="S458" s="1">
         <v>3.37</v>
       </c>
-      <c r="Z458" s="1">
+      <c r="Z458" s="2">
         <f>AA458-0.7116</f>
         <v>-4.2899999999999938E-2</v>
       </c>
@@ -19860,14 +19870,14 @@
       <c r="M459" s="1">
         <v>25</v>
       </c>
-      <c r="R459" s="1">
+      <c r="R459" s="2">
         <f t="shared" si="83"/>
         <v>0.16999999999999993</v>
       </c>
       <c r="S459" s="1">
         <v>3.6</v>
       </c>
-      <c r="Z459" s="1">
+      <c r="Z459" s="2">
         <f t="shared" ref="Z459:Z472" si="84">AA459-0.7116</f>
         <v>1.4800000000000035E-2</v>
       </c>
@@ -19900,14 +19910,14 @@
       <c r="M460" s="1">
         <v>25</v>
       </c>
-      <c r="R460" s="1">
+      <c r="R460" s="2">
         <f t="shared" si="83"/>
         <v>0.19999999999999973</v>
       </c>
       <c r="S460" s="1">
         <v>3.63</v>
       </c>
-      <c r="Z460" s="1">
+      <c r="Z460" s="2">
         <f t="shared" si="84"/>
         <v>-1.0000000000000009E-3</v>
       </c>
@@ -19940,14 +19950,14 @@
       <c r="M461" s="1">
         <v>25</v>
       </c>
-      <c r="R461" s="1">
+      <c r="R461" s="2">
         <f t="shared" si="83"/>
         <v>0.20999999999999996</v>
       </c>
       <c r="S461" s="1">
         <v>3.64</v>
       </c>
-      <c r="Z461" s="1">
+      <c r="Z461" s="2">
         <f t="shared" si="84"/>
         <v>-2.8400000000000092E-2</v>
       </c>
@@ -19980,14 +19990,14 @@
       <c r="M462" s="1">
         <v>25</v>
       </c>
-      <c r="R462" s="1">
+      <c r="R462" s="2">
         <f t="shared" si="83"/>
         <v>0.14999999999999991</v>
       </c>
       <c r="S462" s="1">
         <v>3.58</v>
       </c>
-      <c r="Z462" s="1">
+      <c r="Z462" s="2">
         <f t="shared" si="84"/>
         <v>-1.4999999999999458E-3</v>
       </c>
@@ -20020,14 +20030,14 @@
       <c r="M463" s="1">
         <v>25</v>
       </c>
-      <c r="R463" s="1">
+      <c r="R463" s="2">
         <f t="shared" si="83"/>
         <v>0.25999999999999979</v>
       </c>
       <c r="S463" s="1">
         <v>3.69</v>
       </c>
-      <c r="Z463" s="1">
+      <c r="Z463" s="2">
         <f t="shared" si="84"/>
         <v>-2.4399999999999977E-2</v>
       </c>
@@ -20060,14 +20070,14 @@
       <c r="M464" s="1">
         <v>25</v>
       </c>
-      <c r="R464" s="1">
+      <c r="R464" s="2">
         <f t="shared" si="83"/>
         <v>0.18999999999999995</v>
       </c>
       <c r="S464" s="1">
         <v>3.62</v>
       </c>
-      <c r="Z464" s="1">
+      <c r="Z464" s="2">
         <f t="shared" si="84"/>
         <v>-6.0000000000000053E-3</v>
       </c>
@@ -20100,14 +20110,14 @@
       <c r="M465" s="1">
         <v>25</v>
       </c>
-      <c r="R465" s="1">
+      <c r="R465" s="2">
         <f t="shared" si="83"/>
         <v>0.20999999999999996</v>
       </c>
       <c r="S465" s="1">
         <v>3.64</v>
       </c>
-      <c r="Z465" s="1">
+      <c r="Z465" s="2">
         <f t="shared" si="84"/>
         <v>-5.0800000000000067E-2</v>
       </c>
@@ -20140,14 +20150,14 @@
       <c r="M466" s="1">
         <v>25</v>
       </c>
-      <c r="R466" s="1">
+      <c r="R466" s="2">
         <f t="shared" si="83"/>
         <v>0.20999999999999996</v>
       </c>
       <c r="S466" s="1">
         <v>3.64</v>
       </c>
-      <c r="Z466" s="1">
+      <c r="Z466" s="2">
         <f t="shared" si="84"/>
         <v>-5.0300000000000011E-2</v>
       </c>
@@ -20180,14 +20190,14 @@
       <c r="M467" s="1">
         <v>25</v>
       </c>
-      <c r="R467" s="1">
+      <c r="R467" s="2">
         <f t="shared" si="83"/>
         <v>0.22999999999999998</v>
       </c>
       <c r="S467" s="1">
         <v>3.66</v>
       </c>
-      <c r="Z467" s="1">
+      <c r="Z467" s="2">
         <f t="shared" si="84"/>
         <v>-2.7200000000000002E-2</v>
       </c>
@@ -20220,14 +20230,14 @@
       <c r="M468" s="1">
         <v>25</v>
       </c>
-      <c r="R468" s="1">
+      <c r="R468" s="2">
         <f t="shared" si="83"/>
         <v>0.1599999999999997</v>
       </c>
       <c r="S468" s="1">
         <v>3.59</v>
       </c>
-      <c r="Z468" s="1">
+      <c r="Z468" s="2">
         <f t="shared" si="84"/>
         <v>-4.7000000000000375E-3</v>
       </c>
@@ -20260,14 +20270,14 @@
       <c r="M469" s="1">
         <v>25</v>
       </c>
-      <c r="R469" s="1">
+      <c r="R469" s="2">
         <f t="shared" si="83"/>
         <v>0.21999999999999975</v>
       </c>
       <c r="S469" s="1">
         <v>3.65</v>
       </c>
-      <c r="Z469" s="1">
+      <c r="Z469" s="2">
         <f t="shared" si="84"/>
         <v>-2.3600000000000065E-2</v>
       </c>
@@ -20300,14 +20310,14 @@
       <c r="M470" s="1">
         <v>25</v>
       </c>
-      <c r="R470" s="1">
+      <c r="R470" s="2">
         <f t="shared" si="83"/>
         <v>0.19999999999999973</v>
       </c>
       <c r="S470" s="1">
         <v>3.63</v>
       </c>
-      <c r="Z470" s="1">
+      <c r="Z470" s="2">
         <f t="shared" si="84"/>
         <v>-4.2599999999999971E-2</v>
       </c>
@@ -20340,14 +20350,14 @@
       <c r="M471" s="1">
         <v>25</v>
       </c>
-      <c r="R471" s="1">
+      <c r="R471" s="2">
         <f t="shared" si="83"/>
         <v>0.25</v>
       </c>
       <c r="S471" s="1">
         <v>3.68</v>
       </c>
-      <c r="Z471" s="1">
+      <c r="Z471" s="2">
         <f t="shared" si="84"/>
         <v>-3.8200000000000012E-2</v>
       </c>
@@ -20380,14 +20390,14 @@
       <c r="M472" s="1">
         <v>25</v>
       </c>
-      <c r="R472" s="1">
+      <c r="R472" s="2">
         <f t="shared" si="83"/>
         <v>0.19999999999999973</v>
       </c>
       <c r="S472" s="1">
         <v>3.63</v>
       </c>
-      <c r="Z472" s="1">
+      <c r="Z472" s="2">
         <f t="shared" si="84"/>
         <v>-1.2299999999999978E-2</v>
       </c>
@@ -20420,14 +20430,14 @@
       <c r="M473" s="1">
         <v>30</v>
       </c>
-      <c r="R473" s="1">
+      <c r="R473" s="2">
         <f>S473-3.74</f>
         <v>0.19999999999999973</v>
       </c>
       <c r="S473" s="1">
         <v>3.94</v>
       </c>
-      <c r="Z473" s="4">
+      <c r="Z473" s="2">
         <f>AA473-0.7368</f>
         <v>-3.4400000000000097E-2</v>
       </c>
@@ -20460,14 +20470,14 @@
       <c r="M474" s="1">
         <v>30</v>
       </c>
-      <c r="R474" s="1">
+      <c r="R474" s="2">
         <f t="shared" ref="R474:R488" si="85">S474-3.74</f>
         <v>-0.27</v>
       </c>
       <c r="S474" s="1">
         <v>3.47</v>
       </c>
-      <c r="Z474" s="4">
+      <c r="Z474" s="2">
         <f>AA474-0.7368</f>
         <v>-5.2900000000000058E-2</v>
       </c>
@@ -20500,14 +20510,14 @@
       <c r="M475" s="1">
         <v>30</v>
       </c>
-      <c r="R475" s="1">
+      <c r="R475" s="2">
         <f t="shared" si="85"/>
         <v>0.14999999999999991</v>
       </c>
       <c r="S475" s="1">
         <v>3.89</v>
       </c>
-      <c r="Z475" s="4">
+      <c r="Z475" s="2">
         <f t="shared" ref="Z475:Z488" si="86">AA475-0.7368</f>
         <v>4.4999999999999485E-3</v>
       </c>
@@ -20540,14 +20550,14 @@
       <c r="M476" s="1">
         <v>30</v>
       </c>
-      <c r="R476" s="1">
+      <c r="R476" s="2">
         <f t="shared" si="85"/>
         <v>0.14999999999999991</v>
       </c>
       <c r="S476" s="1">
         <v>3.89</v>
       </c>
-      <c r="Z476" s="4">
+      <c r="Z476" s="2">
         <f t="shared" si="86"/>
         <v>-1.0800000000000032E-2</v>
       </c>
@@ -20580,14 +20590,14 @@
       <c r="M477" s="1">
         <v>30</v>
       </c>
-      <c r="R477" s="1">
+      <c r="R477" s="2">
         <f t="shared" si="85"/>
         <v>0.17999999999999972</v>
       </c>
       <c r="S477" s="1">
         <v>3.92</v>
       </c>
-      <c r="Z477" s="4">
+      <c r="Z477" s="2">
         <f t="shared" si="86"/>
         <v>-2.4000000000000021E-2</v>
       </c>
@@ -20620,14 +20630,14 @@
       <c r="M478" s="1">
         <v>30</v>
       </c>
-      <c r="R478" s="1">
+      <c r="R478" s="2">
         <f t="shared" si="85"/>
         <v>9.9999999999999645E-2</v>
       </c>
       <c r="S478" s="1">
         <v>3.84</v>
       </c>
-      <c r="Z478" s="4">
+      <c r="Z478" s="2">
         <f t="shared" si="86"/>
         <v>-2.9999999999996696E-4</v>
       </c>
@@ -20660,14 +20670,14 @@
       <c r="M479" s="1">
         <v>30</v>
       </c>
-      <c r="R479" s="1">
+      <c r="R479" s="2">
         <f t="shared" si="85"/>
         <v>0.19999999999999973</v>
       </c>
       <c r="S479" s="1">
         <v>3.94</v>
       </c>
-      <c r="Z479" s="4">
+      <c r="Z479" s="2">
         <f t="shared" si="86"/>
         <v>-2.1199999999999997E-2</v>
       </c>
@@ -20700,14 +20710,14 @@
       <c r="M480" s="1">
         <v>30</v>
       </c>
-      <c r="R480" s="1">
+      <c r="R480" s="2">
         <f t="shared" si="85"/>
         <v>0.13999999999999968</v>
       </c>
       <c r="S480" s="1">
         <v>3.88</v>
       </c>
-      <c r="Z480" s="4">
+      <c r="Z480" s="2">
         <f t="shared" si="86"/>
         <v>-6.0000000000000053E-3</v>
       </c>
@@ -20740,14 +20750,14 @@
       <c r="M481" s="1">
         <v>30</v>
       </c>
-      <c r="R481" s="1">
+      <c r="R481" s="2">
         <f t="shared" si="85"/>
         <v>0.13999999999999968</v>
       </c>
       <c r="S481" s="1">
         <v>3.88</v>
       </c>
-      <c r="Z481" s="4">
+      <c r="Z481" s="2">
         <f t="shared" si="86"/>
         <v>-4.3200000000000016E-2</v>
       </c>
@@ -20780,14 +20790,14 @@
       <c r="M482" s="1">
         <v>30</v>
       </c>
-      <c r="R482" s="1">
+      <c r="R482" s="2">
         <f t="shared" si="85"/>
         <v>0.13999999999999968</v>
       </c>
       <c r="S482" s="1">
         <v>3.88</v>
       </c>
-      <c r="Z482" s="4">
+      <c r="Z482" s="2">
         <f t="shared" si="86"/>
         <v>-4.2799999999999949E-2</v>
       </c>
@@ -20820,14 +20830,14 @@
       <c r="M483" s="1">
         <v>30</v>
       </c>
-      <c r="R483" s="1">
+      <c r="R483" s="2">
         <f t="shared" si="85"/>
         <v>0.1599999999999997</v>
       </c>
       <c r="S483" s="1">
         <v>3.9</v>
       </c>
-      <c r="Z483" s="4">
+      <c r="Z483" s="2">
         <f t="shared" si="86"/>
         <v>-2.4499999999999966E-2</v>
       </c>
@@ -20860,14 +20870,14 @@
       <c r="M484" s="1">
         <v>30</v>
       </c>
-      <c r="R484" s="1">
+      <c r="R484" s="2">
         <f t="shared" si="85"/>
         <v>0.11999999999999966</v>
       </c>
       <c r="S484" s="1">
         <v>3.86</v>
       </c>
-      <c r="Z484" s="4">
+      <c r="Z484" s="2">
         <f t="shared" si="86"/>
         <v>-5.9000000000000163E-3</v>
       </c>
@@ -20900,14 +20910,14 @@
       <c r="M485" s="1">
         <v>30</v>
       </c>
-      <c r="R485" s="1">
+      <c r="R485" s="2">
         <f t="shared" si="85"/>
         <v>0.16999999999999993</v>
       </c>
       <c r="S485" s="1">
         <v>3.91</v>
       </c>
-      <c r="Z485" s="4">
+      <c r="Z485" s="2">
         <f t="shared" si="86"/>
         <v>-1.9499999999999962E-2</v>
       </c>
@@ -20940,14 +20950,14 @@
       <c r="M486" s="1">
         <v>30</v>
       </c>
-      <c r="R486" s="1">
+      <c r="R486" s="2">
         <f t="shared" si="85"/>
         <v>0.14999999999999991</v>
       </c>
       <c r="S486" s="1">
         <v>3.89</v>
       </c>
-      <c r="Z486" s="4">
+      <c r="Z486" s="2">
         <f t="shared" si="86"/>
         <v>-3.4700000000000064E-2</v>
       </c>
@@ -20980,14 +20990,14 @@
       <c r="M487" s="1">
         <v>30</v>
       </c>
-      <c r="R487" s="1">
+      <c r="R487" s="2">
         <f t="shared" si="85"/>
         <v>0.19999999999999973</v>
       </c>
       <c r="S487" s="1">
         <v>3.94</v>
       </c>
-      <c r="Z487" s="4">
+      <c r="Z487" s="2">
         <f t="shared" si="86"/>
         <v>-2.9900000000000038E-2</v>
       </c>
@@ -21020,14 +21030,14 @@
       <c r="M488" s="1">
         <v>30</v>
       </c>
-      <c r="R488" s="1">
+      <c r="R488" s="2">
         <f t="shared" si="85"/>
         <v>0.14999999999999991</v>
       </c>
       <c r="S488" s="1">
         <v>3.89</v>
       </c>
-      <c r="Z488" s="4">
+      <c r="Z488" s="2">
         <f t="shared" si="86"/>
         <v>-3.7000000000000366E-3</v>
       </c>
@@ -21060,14 +21070,14 @@
       <c r="M489" s="1">
         <v>0</v>
       </c>
-      <c r="R489" s="1">
+      <c r="R489" s="2">
         <f>S489-1.29</f>
         <v>9.9999999999999867E-2</v>
       </c>
       <c r="S489" s="1">
         <v>1.39</v>
       </c>
-      <c r="T489" s="1">
+      <c r="T489" s="2">
         <f>U489-1.7</f>
         <v>0.40000000000000013</v>
       </c>
@@ -21100,7 +21110,7 @@
       <c r="M490" s="1">
         <v>5</v>
       </c>
-      <c r="R490" s="1">
+      <c r="R490" s="2">
         <f>S490-1.37</f>
         <v>0.22999999999999998</v>
       </c>
@@ -21133,7 +21143,7 @@
       <c r="M491" s="1">
         <v>10</v>
       </c>
-      <c r="R491" s="1">
+      <c r="R491" s="2">
         <f>S491-1.58</f>
         <v>0.25</v>
       </c>
@@ -21166,14 +21176,14 @@
       <c r="M492" s="1">
         <v>0</v>
       </c>
-      <c r="R492" s="1">
+      <c r="R492" s="2">
         <f>S492-1.29</f>
         <v>0.16999999999999993</v>
       </c>
       <c r="S492" s="1">
         <v>1.46</v>
       </c>
-      <c r="T492" s="1">
+      <c r="T492" s="2">
         <f>U492-1.8</f>
         <v>0.59999999999999987</v>
       </c>
@@ -21206,7 +21216,7 @@
       <c r="M493" s="1">
         <v>5</v>
       </c>
-      <c r="R493" s="1">
+      <c r="R493" s="2">
         <f>S493-1.44</f>
         <v>0.22999999999999998</v>
       </c>
@@ -21239,7 +21249,7 @@
       <c r="M494" s="1">
         <v>10</v>
       </c>
-      <c r="R494" s="1">
+      <c r="R494" s="2">
         <f>S494-1.67</f>
         <v>0.24</v>
       </c>
@@ -21272,14 +21282,14 @@
       <c r="M495" s="1">
         <v>0</v>
       </c>
-      <c r="R495" s="1">
+      <c r="R495" s="2">
         <f>S495-1.29</f>
         <v>0.14999999999999991</v>
       </c>
       <c r="S495" s="1">
         <v>1.44</v>
       </c>
-      <c r="T495" s="1">
+      <c r="T495" s="2">
         <f>U495-1.7</f>
         <v>0.8</v>
       </c>
@@ -21312,7 +21322,7 @@
       <c r="M496" s="1">
         <v>5</v>
       </c>
-      <c r="R496" s="1">
+      <c r="R496" s="2">
         <f>S496-1.37</f>
         <v>0.32999999999999985</v>
       </c>
@@ -21345,7 +21355,7 @@
       <c r="M497" s="1">
         <v>10</v>
       </c>
-      <c r="R497" s="1">
+      <c r="R497" s="2">
         <f>S497-1.58</f>
         <v>0.36999999999999988</v>
       </c>
@@ -21378,14 +21388,14 @@
       <c r="M498" s="1">
         <v>0</v>
       </c>
-      <c r="R498" s="1">
+      <c r="R498" s="2">
         <f>S498-1.29</f>
         <v>0.24</v>
       </c>
       <c r="S498" s="1">
         <v>1.53</v>
       </c>
-      <c r="T498" s="1">
+      <c r="T498" s="2">
         <f>U498-1.8</f>
         <v>0.99999999999999978</v>
       </c>
@@ -21418,7 +21428,7 @@
       <c r="M499" s="1">
         <v>5</v>
       </c>
-      <c r="R499" s="1">
+      <c r="R499" s="2">
         <f>S499-1.44</f>
         <v>0.34000000000000008</v>
       </c>
@@ -21451,7 +21461,7 @@
       <c r="M500" s="1">
         <v>10</v>
       </c>
-      <c r="R500" s="1">
+      <c r="R500" s="2">
         <f>S500-1.67</f>
         <v>0.35999999999999988</v>
       </c>
@@ -21484,14 +21494,14 @@
       <c r="M501" s="1">
         <v>0</v>
       </c>
-      <c r="R501" s="1">
+      <c r="R501" s="2">
         <f>S501-1.29</f>
         <v>0.17999999999999994</v>
       </c>
       <c r="S501" s="1">
         <v>1.47</v>
       </c>
-      <c r="T501" s="1">
+      <c r="T501" s="2">
         <f>U501-1.7</f>
         <v>1.0000000000000002</v>
       </c>
@@ -21524,7 +21534,7 @@
       <c r="M502" s="1">
         <v>5</v>
       </c>
-      <c r="R502" s="1">
+      <c r="R502" s="2">
         <f>S502-1.37</f>
         <v>0.34999999999999987</v>
       </c>
@@ -21557,7 +21567,7 @@
       <c r="M503" s="1">
         <v>10</v>
       </c>
-      <c r="R503" s="1">
+      <c r="R503" s="2">
         <f>S503-1.58</f>
         <v>0.37999999999999989</v>
       </c>
@@ -21590,14 +21600,14 @@
       <c r="M504" s="1">
         <v>0</v>
       </c>
-      <c r="R504" s="1">
+      <c r="R504" s="2">
         <f>S504-1.29</f>
         <v>0.28000000000000003</v>
       </c>
       <c r="S504" s="1">
         <v>1.57</v>
       </c>
-      <c r="T504" s="1">
+      <c r="T504" s="2">
         <f>U504-1.8</f>
         <v>0.7</v>
       </c>
@@ -21630,7 +21640,7 @@
       <c r="M505" s="1">
         <v>5</v>
       </c>
-      <c r="R505" s="1">
+      <c r="R505" s="2">
         <f>S505-1.44</f>
         <v>0.37000000000000011</v>
       </c>
@@ -21663,7 +21673,7 @@
       <c r="M506" s="1">
         <v>10</v>
       </c>
-      <c r="R506" s="1">
+      <c r="R506" s="2">
         <f>S506-1.67</f>
         <v>0.35999999999999988</v>
       </c>
@@ -21672,11 +21682,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" scale="43" fitToHeight="12" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+      <mx:PLV Mode="0" OnePage="0" WScale="100"/>
     </ext>
   </extLst>
 </worksheet>

</xml_diff>